<commit_message>
Fixed event for a couple of U20M throws
</commit_message>
<xml_diff>
--- a/2009_CnC_records.xlsx
+++ b/2009_CnC_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A8228A-7F24-4FC4-8267-E051BFCA4E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CED60F-CE82-45AF-B29E-787F16952020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="883" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,12 +32,25 @@
     <definedName name="WOMEN_BY_GROUP" localSheetId="0">Men!$B$257:$J$379</definedName>
     <definedName name="WOMEN_BY_GROUP">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="101716"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3585" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3585" uniqueCount="952">
   <si>
     <t>CAMBRIDGE &amp; COLERIDGE AC</t>
   </si>
@@ -2929,6 +2942,9 @@
   </si>
   <si>
     <t>2:19:55</t>
+  </si>
+  <si>
+    <t>HT6.25K</t>
   </si>
 </sst>
 </file>
@@ -6079,8 +6095,8 @@
   </sheetPr>
   <dimension ref="B1:M1410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="18"/>
@@ -7417,7 +7433,7 @@
         <v>119</v>
       </c>
       <c r="I53" s="103" t="s">
-        <v>856</v>
+        <v>908</v>
       </c>
       <c r="J53" s="35" t="s">
         <v>839</v>
@@ -7448,7 +7464,7 @@
         <v>119</v>
       </c>
       <c r="I54" s="103" t="s">
-        <v>51</v>
+        <v>951</v>
       </c>
       <c r="J54" s="35" t="s">
         <v>839</v>

</xml_diff>

<commit_message>
Fixed U17 Hep event codes
</commit_message>
<xml_diff>
--- a/2009_CnC_records.xlsx
+++ b/2009_CnC_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7346946-D6B0-4672-A020-B5B6A8228B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15400604-648F-46C3-A70A-78C6470A2D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="883" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="883" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Men" sheetId="10" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3585" uniqueCount="952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3587" uniqueCount="954">
   <si>
     <t>CAMBRIDGE &amp; COLERIDGE AC</t>
   </si>
@@ -2737,9 +2737,6 @@
     <t>HT3K</t>
   </si>
   <si>
-    <t>HepW</t>
-  </si>
-  <si>
     <t>Checked Powerof10 for weight</t>
   </si>
   <si>
@@ -2945,6 +2942,15 @@
   </si>
   <si>
     <t>11m08.5s</t>
+  </si>
+  <si>
+    <t>Assuming specific event for U17</t>
+  </si>
+  <si>
+    <t>HepU17W</t>
+  </si>
+  <si>
+    <t>No U15 event code for this so assuming U17 version</t>
   </si>
 </sst>
 </file>
@@ -6095,7 +6101,7 @@
   </sheetPr>
   <dimension ref="B1:M1410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
@@ -6175,7 +6181,7 @@
         <v>825</v>
       </c>
       <c r="K7" s="102" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="8" spans="2:11">
@@ -6708,7 +6714,7 @@
         <v>81</v>
       </c>
       <c r="I27" s="103" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="J27" s="35" t="s">
         <v>838</v>
@@ -6726,7 +6732,7 @@
       </c>
       <c r="D28" s="41"/>
       <c r="E28" s="116" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F28" s="42">
         <v>1975</v>
@@ -6745,7 +6751,7 @@
         <v>839</v>
       </c>
       <c r="M28" s="35" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -6767,7 +6773,7 @@
         <v>699</v>
       </c>
       <c r="I29" s="103" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="J29" s="35" t="s">
         <v>838</v>
@@ -6776,7 +6782,7 @@
         <v>839</v>
       </c>
       <c r="M29" s="35" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -7433,7 +7439,7 @@
         <v>119</v>
       </c>
       <c r="I53" s="103" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="J53" s="35" t="s">
         <v>838</v>
@@ -7464,7 +7470,7 @@
         <v>119</v>
       </c>
       <c r="I54" s="103" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="J54" s="35" t="s">
         <v>838</v>
@@ -8755,7 +8761,7 @@
         <v>172</v>
       </c>
       <c r="E104" s="37" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F104" s="34">
         <v>1990</v>
@@ -8790,7 +8796,7 @@
         <v>123</v>
       </c>
       <c r="I105" s="103" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="J105" s="35" t="s">
         <v>838</v>
@@ -8799,7 +8805,7 @@
         <v>850</v>
       </c>
       <c r="L105" s="35" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="106" spans="2:12">
@@ -8819,7 +8825,7 @@
         <v>701</v>
       </c>
       <c r="I106" s="103" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="J106" s="35" t="s">
         <v>838</v>
@@ -16519,8 +16525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:M1396"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M88" sqref="M88"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M116" sqref="M116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="12.75"/>
@@ -16597,7 +16603,7 @@
         <v>825</v>
       </c>
       <c r="L7" s="102" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="15">
@@ -16804,7 +16810,7 @@
         <v>227</v>
       </c>
       <c r="J15" s="112" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K15" s="84" t="s">
         <v>874</v>
@@ -16833,7 +16839,7 @@
         <v>227</v>
       </c>
       <c r="J16" s="112" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="K16" s="84" t="s">
         <v>874</v>
@@ -17396,7 +17402,7 @@
         <v>489</v>
       </c>
       <c r="J36" s="112" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K36" s="84" t="s">
         <v>874</v>
@@ -17425,7 +17431,7 @@
         <v>703</v>
       </c>
       <c r="J37" s="112" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="K37" s="84" t="s">
         <v>874</v>
@@ -17988,7 +17994,7 @@
         <v>251</v>
       </c>
       <c r="J57" s="112" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K57" s="84" t="s">
         <v>874</v>
@@ -18017,7 +18023,7 @@
         <v>489</v>
       </c>
       <c r="J58" s="112" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K58" s="84" t="s">
         <v>874</v>
@@ -18046,7 +18052,7 @@
         <v>703</v>
       </c>
       <c r="J59" s="112" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="K59" s="84" t="s">
         <v>874</v>
@@ -18055,7 +18061,7 @@
         <v>842</v>
       </c>
       <c r="M59" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="60" spans="2:13" ht="18">
@@ -18078,7 +18084,7 @@
         <v>703</v>
       </c>
       <c r="J60" s="112" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="K60" s="84" t="s">
         <v>874</v>
@@ -18087,7 +18093,7 @@
         <v>842</v>
       </c>
       <c r="M60" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="61" spans="2:13" ht="18">
@@ -18296,7 +18302,7 @@
         <v>842</v>
       </c>
       <c r="M67" s="84" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="68" spans="2:13" ht="18">
@@ -18319,7 +18325,7 @@
         <v>280</v>
       </c>
       <c r="J68" s="112" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="K68" s="84" t="s">
         <v>874</v>
@@ -18328,7 +18334,7 @@
         <v>842</v>
       </c>
       <c r="M68" s="84" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="69" spans="2:13" ht="18">
@@ -18383,13 +18389,16 @@
         <v>282</v>
       </c>
       <c r="J70" s="112" t="s">
-        <v>882</v>
+        <v>952</v>
       </c>
       <c r="K70" s="84" t="s">
         <v>874</v>
       </c>
       <c r="L70" s="84" t="s">
         <v>842</v>
+      </c>
+      <c r="M70" s="84" t="s">
+        <v>951</v>
       </c>
     </row>
     <row r="71" spans="2:13" ht="18">
@@ -18644,7 +18653,7 @@
         <v>251</v>
       </c>
       <c r="J80" s="112" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="K80" s="84" t="s">
         <v>874</v>
@@ -18769,7 +18778,7 @@
         <v>849</v>
       </c>
       <c r="M84" s="84" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="85" spans="2:13" ht="18">
@@ -18833,7 +18842,7 @@
         <v>849</v>
       </c>
       <c r="M86" s="84" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="87" spans="2:13" ht="18">
@@ -18856,7 +18865,7 @@
         <v>296</v>
       </c>
       <c r="J87" s="112" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="K87" s="84" t="s">
         <v>874</v>
@@ -18865,7 +18874,7 @@
         <v>849</v>
       </c>
       <c r="M87" s="84" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="88" spans="2:13" ht="18">
@@ -18897,7 +18906,7 @@
         <v>849</v>
       </c>
       <c r="M88" s="84" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="89" spans="2:13" ht="18">
@@ -18920,13 +18929,16 @@
         <v>282</v>
       </c>
       <c r="J89" s="112" t="s">
-        <v>882</v>
+        <v>952</v>
       </c>
       <c r="K89" s="84" t="s">
         <v>874</v>
       </c>
       <c r="L89" s="84" t="s">
         <v>849</v>
+      </c>
+      <c r="M89" s="84" t="s">
+        <v>953</v>
       </c>
     </row>
     <row r="90" spans="2:13" ht="18">
@@ -19135,7 +19147,7 @@
         <v>704</v>
       </c>
       <c r="J97" s="112" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="K97" s="84" t="s">
         <v>874</v>
@@ -19144,7 +19156,7 @@
         <v>850</v>
       </c>
       <c r="M97" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="98" spans="2:13" ht="18">
@@ -19167,7 +19179,7 @@
         <v>704</v>
       </c>
       <c r="J98" s="112" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="K98" s="84" t="s">
         <v>874</v>
@@ -19176,7 +19188,7 @@
         <v>850</v>
       </c>
       <c r="M98" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="99" spans="2:13" ht="18">
@@ -19286,7 +19298,7 @@
         <v>554</v>
       </c>
       <c r="J102" s="112" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="K102" s="84" t="s">
         <v>874</v>
@@ -19344,7 +19356,7 @@
         <v>541</v>
       </c>
       <c r="J104" s="112" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="K104" s="84" t="s">
         <v>874</v>
@@ -27199,7 +27211,7 @@
         <v>825</v>
       </c>
       <c r="K7" s="102" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="L7" s="22"/>
       <c r="M7" s="23"/>
@@ -27501,7 +27513,7 @@
         <v>838</v>
       </c>
       <c r="K20" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L20" s="43"/>
       <c r="M20" s="71"/>
@@ -27533,7 +27545,7 @@
         <v>838</v>
       </c>
       <c r="K21" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L21" s="43"/>
       <c r="M21" s="71"/>
@@ -27565,7 +27577,7 @@
         <v>838</v>
       </c>
       <c r="K22" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L22" s="43"/>
       <c r="M22" s="71"/>
@@ -27597,7 +27609,7 @@
         <v>838</v>
       </c>
       <c r="K23" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L23" s="43"/>
       <c r="M23" s="71"/>
@@ -27629,7 +27641,7 @@
         <v>838</v>
       </c>
       <c r="K24" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L24" s="43"/>
       <c r="M24" s="71"/>
@@ -27661,7 +27673,7 @@
         <v>838</v>
       </c>
       <c r="K25" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L25" s="43"/>
       <c r="M25" s="71"/>
@@ -27687,13 +27699,13 @@
         <v>747</v>
       </c>
       <c r="I26" s="114" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J26" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K26" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L26" s="43"/>
       <c r="M26" s="71"/>
@@ -27725,10 +27737,10 @@
         <v>838</v>
       </c>
       <c r="K27" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L27" s="40" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="M27" s="71"/>
       <c r="N27" s="44"/>
@@ -27759,7 +27771,7 @@
         <v>838</v>
       </c>
       <c r="K28" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L28" s="43"/>
       <c r="M28" s="71"/>
@@ -27791,7 +27803,7 @@
         <v>838</v>
       </c>
       <c r="K29" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L29" s="43"/>
       <c r="M29" s="71"/>
@@ -27823,7 +27835,7 @@
         <v>838</v>
       </c>
       <c r="K30" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L30" s="43"/>
       <c r="M30" s="71"/>
@@ -27855,7 +27867,7 @@
         <v>838</v>
       </c>
       <c r="K31" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L31" s="43"/>
       <c r="M31" s="71"/>
@@ -27887,10 +27899,10 @@
         <v>838</v>
       </c>
       <c r="K32" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L32" s="40" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="M32" s="71"/>
       <c r="N32" s="44"/>
@@ -27921,7 +27933,7 @@
         <v>838</v>
       </c>
       <c r="K33" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L33" s="43"/>
       <c r="M33" s="71"/>
@@ -27953,7 +27965,7 @@
         <v>838</v>
       </c>
       <c r="K34" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L34" s="44"/>
       <c r="M34" s="42"/>
@@ -27978,13 +27990,13 @@
         <v>752</v>
       </c>
       <c r="I35" s="106" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="J35" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K35" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L35" s="43"/>
       <c r="N35" s="44"/>
@@ -28008,16 +28020,16 @@
         <v>699</v>
       </c>
       <c r="I36" s="106" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="J36" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K36" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L36" s="40" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="N36" s="44"/>
       <c r="O36" s="44"/>
@@ -28047,7 +28059,7 @@
         <v>838</v>
       </c>
       <c r="K37" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L37" s="43"/>
       <c r="M37" s="71"/>
@@ -28063,7 +28075,7 @@
       </c>
       <c r="D38" s="34"/>
       <c r="E38" s="106" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F38" s="71">
         <v>1982</v>
@@ -28079,10 +28091,10 @@
         <v>838</v>
       </c>
       <c r="K38" s="44" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L38" s="40" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="M38" s="71"/>
       <c r="N38" s="44"/>
@@ -28128,7 +28140,7 @@
         <v>838</v>
       </c>
       <c r="K40" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="41" spans="2:15">
@@ -28156,7 +28168,7 @@
         <v>838</v>
       </c>
       <c r="K41" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="42" spans="2:15">
@@ -28184,7 +28196,7 @@
         <v>838</v>
       </c>
       <c r="K42" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="43" spans="2:15">
@@ -28212,7 +28224,7 @@
         <v>838</v>
       </c>
       <c r="K43" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="44" spans="2:15">
@@ -28240,7 +28252,7 @@
         <v>838</v>
       </c>
       <c r="K44" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="45" spans="2:15">
@@ -28268,7 +28280,7 @@
         <v>838</v>
       </c>
       <c r="K45" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="46" spans="2:15">
@@ -28290,13 +28302,13 @@
         <v>19</v>
       </c>
       <c r="I46" s="114" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J46" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K46" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="47" spans="2:15">
@@ -28318,13 +28330,13 @@
         <v>19</v>
       </c>
       <c r="I47" s="114" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="J47" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K47" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="48" spans="2:15">
@@ -28346,13 +28358,13 @@
         <v>774</v>
       </c>
       <c r="I48" s="114" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="J48" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K48" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="49" spans="2:12">
@@ -28380,10 +28392,10 @@
         <v>838</v>
       </c>
       <c r="K49" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="L49" s="40" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="50" spans="2:12">
@@ -28411,7 +28423,7 @@
         <v>838</v>
       </c>
       <c r="K50" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="51" spans="2:12">
@@ -28439,7 +28451,7 @@
         <v>838</v>
       </c>
       <c r="K51" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="52" spans="2:12">
@@ -28467,7 +28479,7 @@
         <v>838</v>
       </c>
       <c r="K52" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="53" spans="2:12">
@@ -28495,7 +28507,7 @@
         <v>838</v>
       </c>
       <c r="K53" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="54" spans="2:12">
@@ -28523,7 +28535,7 @@
         <v>838</v>
       </c>
       <c r="K54" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="55" spans="2:12">
@@ -28551,7 +28563,7 @@
         <v>838</v>
       </c>
       <c r="K55" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="56" spans="2:12">
@@ -28579,7 +28591,7 @@
         <v>838</v>
       </c>
       <c r="K56" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="57" spans="2:12">
@@ -28607,7 +28619,7 @@
         <v>838</v>
       </c>
       <c r="K57" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="58" spans="2:12">
@@ -28635,7 +28647,7 @@
         <v>838</v>
       </c>
       <c r="K58" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="59" spans="2:12">
@@ -28657,13 +28669,13 @@
         <v>33</v>
       </c>
       <c r="I59" s="106" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="J59" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K59" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="60" spans="2:12">
@@ -28675,7 +28687,7 @@
       </c>
       <c r="D60" s="34"/>
       <c r="E60" s="40" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F60" s="34">
         <v>1987</v>
@@ -28691,10 +28703,10 @@
         <v>838</v>
       </c>
       <c r="K60" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="L60" s="37" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="61" spans="2:12">
@@ -28716,16 +28728,16 @@
         <v>733</v>
       </c>
       <c r="I61" s="114" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="J61" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K61" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="L61" s="37" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="62" spans="2:12">
@@ -28753,7 +28765,7 @@
         <v>838</v>
       </c>
       <c r="K62" s="37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="63" spans="2:12">
@@ -28784,7 +28796,7 @@
         <v>838</v>
       </c>
       <c r="K64" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="65" spans="2:18">
@@ -28812,7 +28824,7 @@
         <v>838</v>
       </c>
       <c r="K65" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="66" spans="2:18">
@@ -28840,7 +28852,7 @@
         <v>838</v>
       </c>
       <c r="K66" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="67" spans="2:18">
@@ -28868,7 +28880,7 @@
         <v>838</v>
       </c>
       <c r="K67" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="68" spans="2:18">
@@ -28896,7 +28908,7 @@
         <v>838</v>
       </c>
       <c r="K68" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="69" spans="2:18">
@@ -28924,7 +28936,7 @@
         <v>838</v>
       </c>
       <c r="K69" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="70" spans="2:18">
@@ -28952,7 +28964,7 @@
         <v>838</v>
       </c>
       <c r="K70" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="71" spans="2:18">
@@ -28974,13 +28986,13 @@
         <v>357</v>
       </c>
       <c r="I71" s="114" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J71" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K71" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="72" spans="2:18">
@@ -29002,13 +29014,13 @@
         <v>507</v>
       </c>
       <c r="I72" s="114" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="J72" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K72" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="73" spans="2:18">
@@ -29036,10 +29048,10 @@
         <v>838</v>
       </c>
       <c r="K73" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="L73" s="40" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="74" spans="2:18">
@@ -29067,10 +29079,10 @@
         <v>838</v>
       </c>
       <c r="K74" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="L74" s="40" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="75" spans="2:18">
@@ -29098,7 +29110,7 @@
         <v>838</v>
       </c>
       <c r="K75" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="76" spans="2:18">
@@ -29126,7 +29138,7 @@
         <v>838</v>
       </c>
       <c r="K76" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="77" spans="2:18">
@@ -29154,7 +29166,7 @@
         <v>838</v>
       </c>
       <c r="K77" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="78" spans="2:18">
@@ -29182,7 +29194,7 @@
         <v>838</v>
       </c>
       <c r="K78" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="79" spans="2:18">
@@ -29210,7 +29222,7 @@
         <v>838</v>
       </c>
       <c r="K79" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="R79" s="40"/>
     </row>
@@ -29239,7 +29251,7 @@
         <v>838</v>
       </c>
       <c r="K80" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="81" spans="2:12">
@@ -29267,10 +29279,10 @@
         <v>838</v>
       </c>
       <c r="K81" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="L81" s="37" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="82" spans="2:12">
@@ -29298,7 +29310,7 @@
         <v>838</v>
       </c>
       <c r="K82" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="83" spans="2:12">
@@ -29326,7 +29338,7 @@
         <v>838</v>
       </c>
       <c r="K83" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="84" spans="2:12">
@@ -29348,16 +29360,16 @@
         <v>41</v>
       </c>
       <c r="I84" s="114" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="J84" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K84" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="L84" s="37" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="85" spans="2:12">
@@ -29379,13 +29391,13 @@
         <v>570</v>
       </c>
       <c r="I85" s="114" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="J85" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K85" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="86" spans="2:12">
@@ -29407,13 +29419,13 @@
         <v>570</v>
       </c>
       <c r="I86" s="114" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="J86" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K86" s="37" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="87" spans="2:12">
@@ -29444,7 +29456,7 @@
         <v>838</v>
       </c>
       <c r="K88" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="89" spans="2:12">
@@ -29472,7 +29484,7 @@
         <v>838</v>
       </c>
       <c r="K89" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="90" spans="2:12">
@@ -29500,7 +29512,7 @@
         <v>838</v>
       </c>
       <c r="K90" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="91" spans="2:12">
@@ -29528,7 +29540,7 @@
         <v>838</v>
       </c>
       <c r="K91" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="92" spans="2:12">
@@ -29556,7 +29568,7 @@
         <v>838</v>
       </c>
       <c r="K92" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="93" spans="2:12">
@@ -29584,7 +29596,7 @@
         <v>838</v>
       </c>
       <c r="K93" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="94" spans="2:12">
@@ -29606,13 +29618,13 @@
         <v>357</v>
       </c>
       <c r="I94" s="114" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J94" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K94" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="95" spans="2:12">
@@ -29640,10 +29652,10 @@
         <v>838</v>
       </c>
       <c r="K95" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L95" s="40" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="96" spans="2:12">
@@ -29665,16 +29677,16 @@
         <v>25</v>
       </c>
       <c r="I96" s="103" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="J96" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K96" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L96" s="40" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="97" spans="2:12">
@@ -29702,10 +29714,10 @@
         <v>838</v>
       </c>
       <c r="K97" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L97" s="40" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="98" spans="2:12">
@@ -29733,10 +29745,10 @@
         <v>838</v>
       </c>
       <c r="K98" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L98" s="40" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="99" spans="2:12">
@@ -29764,7 +29776,7 @@
         <v>838</v>
       </c>
       <c r="K99" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="100" spans="2:12">
@@ -29792,7 +29804,7 @@
         <v>838</v>
       </c>
       <c r="K100" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="101" spans="2:12">
@@ -29820,7 +29832,7 @@
         <v>838</v>
       </c>
       <c r="K101" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="102" spans="2:12">
@@ -29848,7 +29860,7 @@
         <v>838</v>
       </c>
       <c r="K102" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="103" spans="2:12">
@@ -29876,7 +29888,7 @@
         <v>838</v>
       </c>
       <c r="K103" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="104" spans="2:12">
@@ -29904,7 +29916,7 @@
         <v>838</v>
       </c>
       <c r="K104" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="105" spans="2:12">
@@ -29932,7 +29944,7 @@
         <v>838</v>
       </c>
       <c r="K105" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="106" spans="2:12">
@@ -29960,7 +29972,7 @@
         <v>838</v>
       </c>
       <c r="K106" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="107" spans="2:12">
@@ -29988,7 +30000,7 @@
         <v>838</v>
       </c>
       <c r="K107" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="108" spans="2:12">
@@ -30016,7 +30028,7 @@
         <v>838</v>
       </c>
       <c r="K108" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="109" spans="2:12">
@@ -30044,7 +30056,7 @@
         <v>838</v>
       </c>
       <c r="K109" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="110" spans="2:12">
@@ -30066,13 +30078,13 @@
         <v>580</v>
       </c>
       <c r="I110" s="103" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="J110" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K110" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="111" spans="2:12">
@@ -30100,7 +30112,7 @@
         <v>838</v>
       </c>
       <c r="K111" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="112" spans="2:12">
@@ -30122,13 +30134,13 @@
         <v>531</v>
       </c>
       <c r="I112" s="103" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="J112" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K112" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="113" spans="2:18">
@@ -30148,16 +30160,16 @@
         <v>730</v>
       </c>
       <c r="I113" s="103" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="J113" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K113" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L113" s="37" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="114" spans="2:18">
@@ -30177,16 +30189,16 @@
         <v>735</v>
       </c>
       <c r="I114" s="114" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="J114" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K114" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L114" s="37" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="115" spans="2:18">
@@ -30218,7 +30230,7 @@
         <v>838</v>
       </c>
       <c r="K116" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="117" spans="2:18">
@@ -30246,7 +30258,7 @@
         <v>838</v>
       </c>
       <c r="K117" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="118" spans="2:18">
@@ -30274,7 +30286,7 @@
         <v>838</v>
       </c>
       <c r="K118" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="119" spans="2:18">
@@ -30302,7 +30314,7 @@
         <v>838</v>
       </c>
       <c r="K119" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="120" spans="2:18">
@@ -30330,7 +30342,7 @@
         <v>838</v>
       </c>
       <c r="K120" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="121" spans="2:18">
@@ -30358,7 +30370,7 @@
         <v>838</v>
       </c>
       <c r="K121" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="122" spans="2:18">
@@ -30380,13 +30392,13 @@
         <v>25</v>
       </c>
       <c r="I122" s="103" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="J122" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K122" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="R122" s="34"/>
     </row>
@@ -30415,10 +30427,10 @@
         <v>838</v>
       </c>
       <c r="K123" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="L123" s="40" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="124" spans="2:18">
@@ -30446,10 +30458,10 @@
         <v>838</v>
       </c>
       <c r="K124" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="L124" s="40" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="125" spans="2:18">
@@ -30461,7 +30473,7 @@
       </c>
       <c r="D125" s="34"/>
       <c r="E125" s="35" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F125" s="34">
         <v>2000</v>
@@ -30471,13 +30483,13 @@
         <v>25</v>
       </c>
       <c r="I125" s="103" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="J125" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K125" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="126" spans="2:18">
@@ -30505,7 +30517,7 @@
         <v>838</v>
       </c>
       <c r="K126" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="127" spans="2:18">
@@ -30533,7 +30545,7 @@
         <v>838</v>
       </c>
       <c r="K127" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="128" spans="2:18">
@@ -30561,7 +30573,7 @@
         <v>838</v>
       </c>
       <c r="K128" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="129" spans="2:12">
@@ -30589,7 +30601,7 @@
         <v>838</v>
       </c>
       <c r="K129" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="130" spans="2:12">
@@ -30617,7 +30629,7 @@
         <v>838</v>
       </c>
       <c r="K130" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="131" spans="2:12">
@@ -30645,7 +30657,7 @@
         <v>838</v>
       </c>
       <c r="K131" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="132" spans="2:12">
@@ -30673,7 +30685,7 @@
         <v>838</v>
       </c>
       <c r="K132" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="133" spans="2:12">
@@ -30701,7 +30713,7 @@
         <v>838</v>
       </c>
       <c r="K133" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="134" spans="2:12">
@@ -30729,7 +30741,7 @@
         <v>838</v>
       </c>
       <c r="K134" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="135" spans="2:12">
@@ -30757,7 +30769,7 @@
         <v>838</v>
       </c>
       <c r="K135" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="136" spans="2:12">
@@ -30779,13 +30791,13 @@
         <v>335</v>
       </c>
       <c r="I136" s="103" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="J136" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K136" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="137" spans="2:12">
@@ -30813,7 +30825,7 @@
         <v>838</v>
       </c>
       <c r="K137" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="138" spans="2:12">
@@ -30835,16 +30847,16 @@
         <v>335</v>
       </c>
       <c r="I138" s="103" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="J138" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K138" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="L138" s="108" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="139" spans="2:12">
@@ -30866,13 +30878,13 @@
         <v>335</v>
       </c>
       <c r="I139" s="103" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="J139" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K139" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="140" spans="2:12">
@@ -30897,10 +30909,10 @@
         <v>838</v>
       </c>
       <c r="K140" s="37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="L140" s="108" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="142" spans="2:12">
@@ -30928,7 +30940,7 @@
         <v>838</v>
       </c>
       <c r="K142" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="143" spans="2:12">
@@ -30956,7 +30968,7 @@
         <v>838</v>
       </c>
       <c r="K143" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="144" spans="2:12">
@@ -30984,7 +30996,7 @@
         <v>838</v>
       </c>
       <c r="K144" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="145" spans="2:11">
@@ -31012,7 +31024,7 @@
         <v>838</v>
       </c>
       <c r="K145" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="146" spans="2:11">
@@ -31040,7 +31052,7 @@
         <v>838</v>
       </c>
       <c r="K146" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="147" spans="2:11">
@@ -31068,7 +31080,7 @@
         <v>838</v>
       </c>
       <c r="K147" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="148" spans="2:11">
@@ -31096,7 +31108,7 @@
         <v>838</v>
       </c>
       <c r="K148" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="149" spans="2:11">
@@ -31124,7 +31136,7 @@
         <v>838</v>
       </c>
       <c r="K149" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="150" spans="2:11">
@@ -31152,7 +31164,7 @@
         <v>838</v>
       </c>
       <c r="K150" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="151" spans="2:11">
@@ -31180,7 +31192,7 @@
         <v>838</v>
       </c>
       <c r="K151" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="152" spans="2:11">
@@ -31208,7 +31220,7 @@
         <v>838</v>
       </c>
       <c r="K152" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="153" spans="2:11">
@@ -31236,7 +31248,7 @@
         <v>838</v>
       </c>
       <c r="K153" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="154" spans="2:11">
@@ -31264,7 +31276,7 @@
         <v>838</v>
       </c>
       <c r="K154" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="155" spans="2:11">
@@ -31292,7 +31304,7 @@
         <v>838</v>
       </c>
       <c r="K155" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="156" spans="2:11">
@@ -31320,7 +31332,7 @@
         <v>838</v>
       </c>
       <c r="K156" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="157" spans="2:11">
@@ -31348,7 +31360,7 @@
         <v>838</v>
       </c>
       <c r="K157" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="158" spans="2:11">
@@ -31376,7 +31388,7 @@
         <v>838</v>
       </c>
       <c r="K158" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="159" spans="2:11">
@@ -31404,7 +31416,7 @@
         <v>838</v>
       </c>
       <c r="K159" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="160" spans="2:11">
@@ -31426,13 +31438,13 @@
         <v>348</v>
       </c>
       <c r="I160" s="103" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="J160" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K160" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="161" spans="2:12">
@@ -31460,7 +31472,7 @@
         <v>838</v>
       </c>
       <c r="K161" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="162" spans="2:12">
@@ -31482,13 +31494,13 @@
         <v>348</v>
       </c>
       <c r="I162" s="103" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="J162" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K162" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="163" spans="2:12">
@@ -31510,13 +31522,13 @@
         <v>530</v>
       </c>
       <c r="I163" s="103" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="J163" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K163" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="164" spans="2:12">
@@ -31538,13 +31550,13 @@
         <v>530</v>
       </c>
       <c r="I164" s="103" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="J164" s="44" t="s">
         <v>838</v>
       </c>
       <c r="K164" s="37" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="165" spans="2:12">
@@ -31572,13 +31584,13 @@
         <v>530</v>
       </c>
       <c r="I166" s="103" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="J166" s="35" t="s">
         <v>838</v>
       </c>
       <c r="K166" s="35" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="167" spans="2:12">
@@ -31600,13 +31612,13 @@
         <v>530</v>
       </c>
       <c r="I167" s="103" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="J167" s="35" t="s">
         <v>838</v>
       </c>
       <c r="K167" s="35" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="168" spans="2:12">
@@ -31630,16 +31642,16 @@
         <v>530</v>
       </c>
       <c r="I168" s="103" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="J168" s="35" t="s">
         <v>838</v>
       </c>
       <c r="K168" s="35" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="L168" s="37" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="169" spans="2:12">
@@ -31661,13 +31673,13 @@
         <v>530</v>
       </c>
       <c r="I169" s="103" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="J169" s="35" t="s">
         <v>838</v>
       </c>
       <c r="K169" s="35" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="170" spans="2:12">
@@ -31695,7 +31707,7 @@
         <v>838</v>
       </c>
       <c r="K170" s="35" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="171" spans="2:12">
@@ -31723,7 +31735,7 @@
         <v>838</v>
       </c>
       <c r="K171" s="35" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="172" spans="2:12">
@@ -31751,7 +31763,7 @@
         <v>838</v>
       </c>
       <c r="K172" s="35" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="173" spans="2:12">
@@ -31779,7 +31791,7 @@
         <v>838</v>
       </c>
       <c r="K173" s="35" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="174" spans="2:12">
@@ -31801,13 +31813,13 @@
         <v>348</v>
       </c>
       <c r="I174" s="103" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="J174" s="35" t="s">
         <v>838</v>
       </c>
       <c r="K174" s="35" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="175" spans="2:12">
@@ -31842,7 +31854,7 @@
         <v>838</v>
       </c>
       <c r="K176" s="35" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="177" spans="2:11">
@@ -31864,13 +31876,13 @@
         <v>664</v>
       </c>
       <c r="I177" s="103" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J177" s="35" t="s">
         <v>838</v>
       </c>
       <c r="K177" s="35" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="179" spans="2:11">
@@ -31898,7 +31910,7 @@
         <v>838</v>
       </c>
       <c r="K179" s="35" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="181" spans="2:11">
@@ -37566,7 +37578,7 @@
         <v>825</v>
       </c>
       <c r="J7" s="102" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="10.15" customHeight="1">
@@ -37601,7 +37613,7 @@
         <v>874</v>
       </c>
       <c r="J9" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="18">
@@ -37628,7 +37640,7 @@
         <v>874</v>
       </c>
       <c r="J10" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="18">
@@ -37655,7 +37667,7 @@
         <v>874</v>
       </c>
       <c r="J11" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="18">
@@ -37682,7 +37694,7 @@
         <v>874</v>
       </c>
       <c r="J12" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="18">
@@ -37709,7 +37721,7 @@
         <v>874</v>
       </c>
       <c r="J13" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="18">
@@ -37736,7 +37748,7 @@
         <v>874</v>
       </c>
       <c r="J14" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="18">
@@ -37757,13 +37769,13 @@
         <v>402</v>
       </c>
       <c r="H15" s="112" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="I15" t="s">
         <v>874</v>
       </c>
       <c r="J15" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="18">
@@ -37784,13 +37796,13 @@
         <v>211</v>
       </c>
       <c r="H16" s="112" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="I16" t="s">
         <v>874</v>
       </c>
       <c r="J16" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="18">
@@ -37811,13 +37823,13 @@
         <v>211</v>
       </c>
       <c r="H17" s="112" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="I17" t="s">
         <v>874</v>
       </c>
       <c r="J17" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="18">
@@ -37844,7 +37856,7 @@
         <v>874</v>
       </c>
       <c r="J18" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="18">
@@ -37871,7 +37883,7 @@
         <v>874</v>
       </c>
       <c r="J19" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="18">
@@ -37898,7 +37910,7 @@
         <v>874</v>
       </c>
       <c r="J20" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="18">
@@ -37925,7 +37937,7 @@
         <v>874</v>
       </c>
       <c r="J21" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="18">
@@ -37952,7 +37964,7 @@
         <v>874</v>
       </c>
       <c r="J22" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="18">
@@ -37979,7 +37991,7 @@
         <v>874</v>
       </c>
       <c r="J23" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="18">
@@ -38006,7 +38018,7 @@
         <v>874</v>
       </c>
       <c r="J24" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="18">
@@ -38033,7 +38045,7 @@
         <v>874</v>
       </c>
       <c r="J25" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="18">
@@ -38060,7 +38072,7 @@
         <v>874</v>
       </c>
       <c r="J26" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="18">
@@ -38081,13 +38093,13 @@
         <v>600</v>
       </c>
       <c r="H27" s="108" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I27" t="s">
         <v>874</v>
       </c>
       <c r="J27" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="18">
@@ -38108,13 +38120,13 @@
         <v>754</v>
       </c>
       <c r="H28" s="108" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="I28" t="s">
         <v>874</v>
       </c>
       <c r="J28" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="18">
@@ -38149,7 +38161,7 @@
         <v>874</v>
       </c>
       <c r="J30" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="18">
@@ -38176,7 +38188,7 @@
         <v>874</v>
       </c>
       <c r="J31" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="18">
@@ -38203,7 +38215,7 @@
         <v>874</v>
       </c>
       <c r="J32" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="18">
@@ -38230,7 +38242,7 @@
         <v>874</v>
       </c>
       <c r="J33" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="18">
@@ -38257,7 +38269,7 @@
         <v>874</v>
       </c>
       <c r="J34" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="18">
@@ -38284,7 +38296,7 @@
         <v>874</v>
       </c>
       <c r="J35" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="18">
@@ -38305,13 +38317,13 @@
         <v>402</v>
       </c>
       <c r="H36" s="112" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="I36" t="s">
         <v>874</v>
       </c>
       <c r="J36" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="18">
@@ -38332,13 +38344,13 @@
         <v>212</v>
       </c>
       <c r="H37" s="112" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="I37" t="s">
         <v>874</v>
       </c>
       <c r="J37" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="18">
@@ -38359,13 +38371,13 @@
         <v>212</v>
       </c>
       <c r="H38" s="112" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="I38" t="s">
         <v>874</v>
       </c>
       <c r="J38" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="18">
@@ -38386,13 +38398,13 @@
         <v>212</v>
       </c>
       <c r="H39" s="108" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="I39" t="s">
         <v>874</v>
       </c>
       <c r="J39" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="40" spans="2:10" ht="18">
@@ -38419,7 +38431,7 @@
         <v>874</v>
       </c>
       <c r="J40" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="41" spans="2:10" ht="18">
@@ -38446,7 +38458,7 @@
         <v>874</v>
       </c>
       <c r="J41" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="42" spans="2:10" ht="18">
@@ -38473,7 +38485,7 @@
         <v>874</v>
       </c>
       <c r="J42" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="18">
@@ -38500,7 +38512,7 @@
         <v>874</v>
       </c>
       <c r="J43" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="18">
@@ -38527,7 +38539,7 @@
         <v>874</v>
       </c>
       <c r="J44" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="45" spans="2:10" ht="18">
@@ -38554,7 +38566,7 @@
         <v>874</v>
       </c>
       <c r="J45" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="18">
@@ -38581,7 +38593,7 @@
         <v>874</v>
       </c>
       <c r="J46" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="18">
@@ -38608,7 +38620,7 @@
         <v>874</v>
       </c>
       <c r="J47" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="18">
@@ -38635,7 +38647,7 @@
         <v>874</v>
       </c>
       <c r="J48" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="13.9" customHeight="1">
@@ -38671,7 +38683,7 @@
         <v>874</v>
       </c>
       <c r="J50" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="18">
@@ -38698,7 +38710,7 @@
         <v>874</v>
       </c>
       <c r="J51" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="18">
@@ -38725,7 +38737,7 @@
         <v>874</v>
       </c>
       <c r="J52" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="18">
@@ -38752,7 +38764,7 @@
         <v>874</v>
       </c>
       <c r="J53" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="18">
@@ -38779,7 +38791,7 @@
         <v>874</v>
       </c>
       <c r="J54" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="18">
@@ -38806,7 +38818,7 @@
         <v>874</v>
       </c>
       <c r="J55" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="56" spans="2:10" s="33" customFormat="1" ht="18">
@@ -38827,13 +38839,13 @@
         <v>209</v>
       </c>
       <c r="H56" s="112" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="I56" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J56" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="18">
@@ -38854,13 +38866,13 @@
         <v>402</v>
       </c>
       <c r="H57" s="108" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I57" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J57" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="58" spans="2:10" ht="18">
@@ -38881,13 +38893,13 @@
         <v>212</v>
       </c>
       <c r="H58" s="112" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="I58" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J58" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="59" spans="2:10" ht="18">
@@ -38908,13 +38920,13 @@
         <v>212</v>
       </c>
       <c r="H59" s="112" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="I59" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J59" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="60" spans="2:10" ht="18">
@@ -38935,13 +38947,13 @@
         <v>212</v>
       </c>
       <c r="H60" s="108" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="I60" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J60" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="61" spans="2:10" ht="18">
@@ -38968,7 +38980,7 @@
         <v>874</v>
       </c>
       <c r="J61" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="62" spans="2:10" ht="18">
@@ -38995,7 +39007,7 @@
         <v>874</v>
       </c>
       <c r="J62" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="63" spans="2:10" ht="18">
@@ -39022,7 +39034,7 @@
         <v>874</v>
       </c>
       <c r="J63" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="64" spans="2:10" ht="18">
@@ -39049,7 +39061,7 @@
         <v>874</v>
       </c>
       <c r="J64" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="65" spans="2:11" ht="18">
@@ -39076,7 +39088,7 @@
         <v>874</v>
       </c>
       <c r="J65" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="66" spans="2:11" ht="18">
@@ -39103,7 +39115,7 @@
         <v>874</v>
       </c>
       <c r="J66" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="67" spans="2:11" ht="17.45" customHeight="1">
@@ -39139,7 +39151,7 @@
         <v>874</v>
       </c>
       <c r="J68" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="69" spans="2:11" ht="17.45" customHeight="1">
@@ -39166,7 +39178,7 @@
         <v>874</v>
       </c>
       <c r="J69" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="70" spans="2:11" ht="18">
@@ -39193,7 +39205,7 @@
         <v>874</v>
       </c>
       <c r="J70" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="71" spans="2:11" ht="18">
@@ -39220,7 +39232,7 @@
         <v>874</v>
       </c>
       <c r="J71" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="72" spans="2:11" ht="18">
@@ -39247,7 +39259,7 @@
         <v>874</v>
       </c>
       <c r="J72" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="73" spans="2:11" ht="18">
@@ -39274,7 +39286,7 @@
         <v>874</v>
       </c>
       <c r="J73" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="74" spans="2:11" ht="18">
@@ -39295,13 +39307,13 @@
         <v>209</v>
       </c>
       <c r="H74" s="112" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="I74" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J74" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="75" spans="2:11" ht="18">
@@ -39328,7 +39340,7 @@
         <v>874</v>
       </c>
       <c r="J75" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="76" spans="2:11" ht="18">
@@ -39355,7 +39367,7 @@
         <v>874</v>
       </c>
       <c r="J76" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="77" spans="2:11" ht="18">
@@ -39376,13 +39388,13 @@
         <v>223</v>
       </c>
       <c r="H77" s="112" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="I77" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J77" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="78" spans="2:11" ht="18">
@@ -39409,7 +39421,7 @@
         <v>874</v>
       </c>
       <c r="J78" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="79" spans="2:11" ht="18">
@@ -39436,10 +39448,10 @@
         <v>874</v>
       </c>
       <c r="J79" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="K79" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="80" spans="2:11" ht="18">
@@ -39466,10 +39478,10 @@
         <v>874</v>
       </c>
       <c r="J80" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="K80" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="81" spans="2:10" ht="18">
@@ -39496,7 +39508,7 @@
         <v>874</v>
       </c>
       <c r="J81" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="82" spans="2:10" ht="18">
@@ -39523,7 +39535,7 @@
         <v>874</v>
       </c>
       <c r="J82" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="83" spans="2:10" ht="18">
@@ -39544,13 +39556,13 @@
         <v>402</v>
       </c>
       <c r="H83" s="108" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I83" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J83" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="84" spans="2:10" ht="18">
@@ -39585,7 +39597,7 @@
         <v>874</v>
       </c>
       <c r="J85" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="86" spans="2:10" ht="18">
@@ -39612,7 +39624,7 @@
         <v>874</v>
       </c>
       <c r="J86" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="87" spans="2:10" ht="18">
@@ -39639,7 +39651,7 @@
         <v>874</v>
       </c>
       <c r="J87" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="88" spans="2:10" ht="18">
@@ -39666,7 +39678,7 @@
         <v>874</v>
       </c>
       <c r="J88" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="89" spans="2:10" ht="18">
@@ -39693,7 +39705,7 @@
         <v>874</v>
       </c>
       <c r="J89" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="90" spans="2:10" ht="18">
@@ -39720,7 +39732,7 @@
         <v>874</v>
       </c>
       <c r="J90" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="91" spans="2:10" ht="18">
@@ -39747,7 +39759,7 @@
         <v>874</v>
       </c>
       <c r="J91" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="92" spans="2:10" ht="18">
@@ -39774,7 +39786,7 @@
         <v>874</v>
       </c>
       <c r="J92" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="93" spans="2:10" ht="18">
@@ -39801,7 +39813,7 @@
         <v>874</v>
       </c>
       <c r="J93" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="94" spans="2:10" ht="18">
@@ -39828,7 +39840,7 @@
         <v>874</v>
       </c>
       <c r="J94" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="95" spans="2:10" ht="18">
@@ -39849,13 +39861,13 @@
         <v>223</v>
       </c>
       <c r="H95" s="112" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="I95" t="s">
         <v>874</v>
       </c>
       <c r="J95" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="96" spans="2:10" ht="18">
@@ -39882,7 +39894,7 @@
         <v>874</v>
       </c>
       <c r="J96" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="97" spans="2:11" ht="18">
@@ -39909,7 +39921,7 @@
         <v>874</v>
       </c>
       <c r="J97" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="98" spans="2:11" ht="18">
@@ -39936,7 +39948,7 @@
         <v>874</v>
       </c>
       <c r="J98" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="99" spans="2:11" ht="18">
@@ -39963,7 +39975,7 @@
         <v>874</v>
       </c>
       <c r="J99" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="100" spans="2:11" ht="18">
@@ -39990,7 +40002,7 @@
         <v>874</v>
       </c>
       <c r="J100" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="101" spans="2:11" ht="18">
@@ -40017,7 +40029,7 @@
         <v>874</v>
       </c>
       <c r="J101" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="102" spans="2:11" ht="18">
@@ -40038,16 +40050,16 @@
         <v>223</v>
       </c>
       <c r="H102" s="112" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I102" t="s">
         <v>874</v>
       </c>
       <c r="J102" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K102" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="103" spans="2:11" ht="18">
@@ -40068,13 +40080,13 @@
         <v>402</v>
       </c>
       <c r="H103" s="112" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="I103" t="s">
         <v>874</v>
       </c>
       <c r="J103" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="104" spans="2:11" ht="18">
@@ -40095,13 +40107,13 @@
         <v>755</v>
       </c>
       <c r="H104" s="112" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I104" t="s">
         <v>874</v>
       </c>
       <c r="J104" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="105" spans="2:11" ht="18">
@@ -40122,13 +40134,13 @@
         <v>402</v>
       </c>
       <c r="H105" s="112" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="I105" t="s">
         <v>874</v>
       </c>
       <c r="J105" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="106" spans="2:11" ht="18">
@@ -40149,13 +40161,13 @@
         <v>755</v>
       </c>
       <c r="H106" s="112" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="I106" t="s">
         <v>874</v>
       </c>
       <c r="J106" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="107" spans="2:11" ht="18">
@@ -40192,7 +40204,7 @@
         <v>874</v>
       </c>
       <c r="J108" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="109" spans="2:11" ht="18.75" thickBot="1">
@@ -40219,7 +40231,7 @@
         <v>874</v>
       </c>
       <c r="J109" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="110" spans="2:11" ht="21.6" customHeight="1" thickBot="1">
@@ -40246,7 +40258,7 @@
         <v>874</v>
       </c>
       <c r="J110" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="111" spans="2:11" ht="18">
@@ -40273,7 +40285,7 @@
         <v>874</v>
       </c>
       <c r="J111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="112" spans="2:11" ht="18">
@@ -40300,7 +40312,7 @@
         <v>874</v>
       </c>
       <c r="J112" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="113" spans="2:11" ht="18">
@@ -40327,7 +40339,7 @@
         <v>874</v>
       </c>
       <c r="J113" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="114" spans="2:11" ht="18">
@@ -40354,7 +40366,7 @@
         <v>874</v>
       </c>
       <c r="J114" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="115" spans="2:11" ht="18">
@@ -40381,7 +40393,7 @@
         <v>874</v>
       </c>
       <c r="J115" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="116" spans="2:11" ht="18">
@@ -40402,13 +40414,13 @@
         <v>741</v>
       </c>
       <c r="H116" s="112" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="I116" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J116" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="117" spans="2:11" ht="18">
@@ -40435,7 +40447,7 @@
         <v>874</v>
       </c>
       <c r="J117" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="118" spans="2:11" ht="18">
@@ -40462,7 +40474,7 @@
         <v>874</v>
       </c>
       <c r="J118" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="119" spans="2:11" ht="18">
@@ -40489,7 +40501,7 @@
         <v>874</v>
       </c>
       <c r="J119" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="120" spans="2:11" ht="18">
@@ -40516,7 +40528,7 @@
         <v>874</v>
       </c>
       <c r="J120" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="121" spans="2:11" ht="18">
@@ -40543,7 +40555,7 @@
         <v>874</v>
       </c>
       <c r="J121" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="122" spans="2:11" ht="18">
@@ -40570,7 +40582,7 @@
         <v>874</v>
       </c>
       <c r="J122" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="123" spans="2:11" ht="18">
@@ -40591,16 +40603,16 @@
         <v>741</v>
       </c>
       <c r="H123" s="112" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="I123" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J123" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K123" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="124" spans="2:11" ht="18">
@@ -40621,16 +40633,16 @@
         <v>741</v>
       </c>
       <c r="H124" s="112" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I124" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J124" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K124" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="125" spans="2:11" ht="18">
@@ -40655,10 +40667,10 @@
         <v>874</v>
       </c>
       <c r="J125" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K125" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="126" spans="2:11" ht="18">
@@ -40695,7 +40707,7 @@
         <v>874</v>
       </c>
       <c r="J127" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="128" spans="2:11" ht="18">
@@ -40722,7 +40734,7 @@
         <v>874</v>
       </c>
       <c r="J128" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="129" spans="2:10" ht="18">
@@ -40749,7 +40761,7 @@
         <v>874</v>
       </c>
       <c r="J129" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="130" spans="2:10" ht="18">
@@ -40776,7 +40788,7 @@
         <v>874</v>
       </c>
       <c r="J130" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="131" spans="2:10" ht="18">
@@ -40803,7 +40815,7 @@
         <v>874</v>
       </c>
       <c r="J131" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="132" spans="2:10" ht="18">
@@ -40815,7 +40827,7 @@
       </c>
       <c r="D132" s="35"/>
       <c r="E132" s="40" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F132" s="34">
         <v>2003</v>
@@ -40830,7 +40842,7 @@
         <v>874</v>
       </c>
       <c r="J132" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="133" spans="2:10" ht="18">
@@ -40851,13 +40863,13 @@
         <v>423</v>
       </c>
       <c r="H133" s="112" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="I133" s="84" t="s">
         <v>874</v>
       </c>
       <c r="J133" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="134" spans="2:10" ht="18">
@@ -40884,7 +40896,7 @@
         <v>874</v>
       </c>
       <c r="J134" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="135" spans="2:10" ht="18">
@@ -40911,7 +40923,7 @@
         <v>874</v>
       </c>
       <c r="J135" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="136" spans="2:10" ht="18">
@@ -40938,7 +40950,7 @@
         <v>874</v>
       </c>
       <c r="J136" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="137" spans="2:10" ht="18">
@@ -40965,7 +40977,7 @@
         <v>874</v>
       </c>
       <c r="J137" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="138" spans="2:10" ht="18">
@@ -40992,7 +41004,7 @@
         <v>874</v>
       </c>
       <c r="J138" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="139" spans="2:10" ht="18">
@@ -41019,7 +41031,7 @@
         <v>874</v>
       </c>
       <c r="J139" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="140" spans="2:10" ht="18">
@@ -41046,7 +41058,7 @@
         <v>874</v>
       </c>
       <c r="J140" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="141" spans="2:10" ht="18">
@@ -41082,7 +41094,7 @@
         <v>874</v>
       </c>
       <c r="J142" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="143" spans="2:10" ht="18">
@@ -41109,7 +41121,7 @@
         <v>874</v>
       </c>
       <c r="J143" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="144" spans="2:10" ht="18.75" thickBot="1">
@@ -41136,7 +41148,7 @@
         <v>874</v>
       </c>
       <c r="J144" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="145" spans="2:10" ht="21" customHeight="1" thickBot="1">
@@ -41163,7 +41175,7 @@
         <v>874</v>
       </c>
       <c r="J145" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="146" spans="2:10" ht="18">
@@ -41190,7 +41202,7 @@
         <v>874</v>
       </c>
       <c r="J146" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="147" spans="2:10" ht="18">
@@ -41217,7 +41229,7 @@
         <v>874</v>
       </c>
       <c r="J147" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="148" spans="2:10" ht="18">
@@ -41244,7 +41256,7 @@
         <v>874</v>
       </c>
       <c r="J148" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="149" spans="2:10" ht="18">
@@ -41271,7 +41283,7 @@
         <v>874</v>
       </c>
       <c r="J149" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="150" spans="2:10" ht="18">
@@ -41298,7 +41310,7 @@
         <v>874</v>
       </c>
       <c r="J150" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="151" spans="2:10" ht="20.25">

</xml_diff>

<commit_message>
Categorised hammer throws. Currently excluding one new event as runbritain request just hanging, so can only use cached results
</commit_message>
<xml_diff>
--- a/2009_CnC_records.xlsx
+++ b/2009_CnC_records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C4F4EB-351E-4703-9BF9-DFFF68F89319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9E2CD1-AD37-40C2-8448-931B264C743B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="883" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="883" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Men" sheetId="10" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3601" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3598" uniqueCount="965">
   <si>
     <t>CAMBRIDGE &amp; COLERIDGE AC</t>
   </si>
@@ -2881,9 +2881,6 @@
     <t>PenIM35</t>
   </si>
   <si>
-    <t>Event code from po10</t>
-  </si>
-  <si>
     <t>75HU13M</t>
   </si>
   <si>
@@ -2984,6 +2981,9 @@
   </si>
   <si>
     <t>Looks like obsolete hurdle height</t>
+  </si>
+  <si>
+    <t>Skipping this because PenIM35 age-group specific, also listed there</t>
   </si>
 </sst>
 </file>
@@ -6141,25 +6141,25 @@
   </sheetPr>
   <dimension ref="B1:M1410"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29:K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="35" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="3.5703125" style="35" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="37" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="34" customWidth="1"/>
+    <col min="4" max="4" width="3.5546875" style="35" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="37" customWidth="1"/>
     <col min="6" max="6" width="14" style="34" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="34" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" style="37" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="103" customWidth="1"/>
-    <col min="10" max="16384" width="12.140625" style="35"/>
+    <col min="7" max="7" width="3.6640625" style="34" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" style="37" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" style="103" customWidth="1"/>
+    <col min="10" max="16384" width="12.109375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="32.25">
+    <row r="1" spans="2:11" ht="31.8">
       <c r="C1" s="35"/>
       <c r="E1" s="52" t="s">
         <v>0</v>
@@ -6173,7 +6173,7 @@
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" spans="2:11" ht="32.25">
+    <row r="3" spans="2:11" ht="31.8">
       <c r="E3" s="53" t="s">
         <v>1</v>
       </c>
@@ -6182,7 +6182,7 @@
     <row r="4" spans="2:11" ht="7.5" customHeight="1">
       <c r="E4" s="51"/>
     </row>
-    <row r="5" spans="2:11" ht="32.25">
+    <row r="5" spans="2:11" ht="31.8">
       <c r="B5" s="98" t="s">
         <v>759</v>
       </c>
@@ -6193,10 +6193,10 @@
         <v>764</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="23.45" customHeight="1">
+    <row r="6" spans="2:11" ht="23.4" customHeight="1">
       <c r="E6" s="39"/>
     </row>
-    <row r="7" spans="2:11" ht="18.75">
+    <row r="7" spans="2:11">
       <c r="B7" s="20" t="s">
         <v>3</v>
       </c>
@@ -6772,7 +6772,7 @@
       </c>
       <c r="D28" s="41"/>
       <c r="E28" s="116" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F28" s="42">
         <v>1975</v>
@@ -6791,7 +6791,7 @@
         <v>835</v>
       </c>
       <c r="M28" s="35" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -6812,17 +6812,8 @@
       <c r="H29" s="44" t="s">
         <v>696</v>
       </c>
-      <c r="I29" s="103" t="s">
-        <v>929</v>
-      </c>
-      <c r="J29" s="35" t="s">
-        <v>834</v>
-      </c>
-      <c r="K29" s="35" t="s">
-        <v>835</v>
-      </c>
-      <c r="M29" s="35" t="s">
-        <v>930</v>
+      <c r="M29" s="108" t="s">
+        <v>964</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -7012,7 +7003,7 @@
       </c>
       <c r="D37" s="41"/>
       <c r="E37" s="40" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F37" s="42">
         <v>2007</v>
@@ -7031,7 +7022,7 @@
         <v>614</v>
       </c>
       <c r="M37" s="35" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="38" spans="2:13">
@@ -7513,7 +7504,7 @@
         <v>119</v>
       </c>
       <c r="I54" s="103" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="J54" s="35" t="s">
         <v>834</v>
@@ -8804,7 +8795,7 @@
         <v>172</v>
       </c>
       <c r="E104" s="37" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F104" s="34">
         <v>1990</v>
@@ -8839,7 +8830,7 @@
         <v>123</v>
       </c>
       <c r="I105" s="103" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="J105" s="35" t="s">
         <v>834</v>
@@ -8848,7 +8839,7 @@
         <v>846</v>
       </c>
       <c r="L105" s="35" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="106" spans="2:12">
@@ -8868,7 +8859,7 @@
         <v>698</v>
       </c>
       <c r="I106" s="103" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="J106" s="35" t="s">
         <v>834</v>
@@ -9252,34 +9243,34 @@
     <row r="122" spans="2:12">
       <c r="G122" s="35"/>
     </row>
-    <row r="123" spans="2:12" ht="32.25">
+    <row r="123" spans="2:12" ht="31.8">
       <c r="C123" s="35"/>
       <c r="E123" s="52"/>
       <c r="F123" s="36"/>
       <c r="G123" s="36"/>
     </row>
-    <row r="124" spans="2:12" ht="22.5">
+    <row r="124" spans="2:12" ht="22.2">
       <c r="D124" s="38"/>
       <c r="E124" s="50"/>
       <c r="F124" s="36"/>
       <c r="G124" s="36"/>
     </row>
-    <row r="125" spans="2:12" ht="32.25">
+    <row r="125" spans="2:12" ht="31.8">
       <c r="E125" s="53"/>
       <c r="F125" s="37"/>
     </row>
-    <row r="126" spans="2:12" ht="13.15" customHeight="1">
+    <row r="126" spans="2:12" ht="13.2" customHeight="1">
       <c r="E126" s="53"/>
       <c r="F126" s="37"/>
       <c r="I126" s="105"/>
     </row>
-    <row r="127" spans="2:12" ht="28.15" customHeight="1">
+    <row r="127" spans="2:12" ht="28.2" customHeight="1">
       <c r="B127" s="98"/>
       <c r="D127" s="46"/>
       <c r="E127" s="97"/>
       <c r="H127" s="101"/>
     </row>
-    <row r="129" spans="2:8" ht="18.75">
+    <row r="129" spans="2:8">
       <c r="B129" s="20"/>
       <c r="C129" s="21"/>
       <c r="D129" s="20"/>
@@ -10105,7 +10096,7 @@
     <row r="316" spans="5:11">
       <c r="E316" s="40"/>
     </row>
-    <row r="322" spans="2:8" ht="18.75">
+    <row r="322" spans="2:8">
       <c r="B322" s="20"/>
       <c r="C322" s="21"/>
       <c r="D322" s="20"/>
@@ -16572,41 +16563,41 @@
       <selection activeCell="M58" sqref="M58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="3.28515625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="3.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="29" style="7" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="108"/>
+    <col min="10" max="10" width="16.44140625" style="108"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="32.25">
+    <row r="1" spans="2:12" ht="31.8">
       <c r="F1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="2:12" ht="4.9000000000000004" customHeight="1">
+    <row r="2" spans="2:12" ht="4.95" customHeight="1">
       <c r="E2" s="30"/>
       <c r="F2" s="11"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="2:12" ht="32.25">
+    <row r="3" spans="2:12" ht="31.8">
       <c r="F3" s="69" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="14.45" customHeight="1">
+    <row r="4" spans="2:12" ht="14.4" customHeight="1">
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="2:12" ht="25.5">
+    <row r="5" spans="2:12" ht="24.6">
       <c r="B5" s="98" t="s">
         <v>759</v>
       </c>
@@ -16620,7 +16611,7 @@
     <row r="6" spans="2:12" ht="18" customHeight="1">
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="2:12" s="28" customFormat="1" ht="20.25">
+    <row r="7" spans="2:12" s="28" customFormat="1" ht="20.399999999999999">
       <c r="B7" s="25" t="s">
         <v>3</v>
       </c>
@@ -16659,7 +16650,7 @@
       <c r="H8" s="15"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="2:12" ht="18">
+    <row r="9" spans="2:12" ht="17.399999999999999">
       <c r="B9" s="35" t="s">
         <v>8</v>
       </c>
@@ -16688,7 +16679,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="18">
+    <row r="10" spans="2:12" ht="17.399999999999999">
       <c r="B10" s="35" t="s">
         <v>11</v>
       </c>
@@ -16717,7 +16708,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="18">
+    <row r="11" spans="2:12" ht="17.399999999999999">
       <c r="B11" s="35" t="s">
         <v>13</v>
       </c>
@@ -16746,7 +16737,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="18">
+    <row r="12" spans="2:12" ht="17.399999999999999">
       <c r="B12" s="35" t="s">
         <v>16</v>
       </c>
@@ -16775,7 +16766,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="18">
+    <row r="13" spans="2:12" ht="17.399999999999999">
       <c r="B13" s="35" t="s">
         <v>398</v>
       </c>
@@ -16804,7 +16795,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="18">
+    <row r="14" spans="2:12" ht="17.399999999999999">
       <c r="B14" s="35" t="s">
         <v>485</v>
       </c>
@@ -16833,7 +16824,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="18">
+    <row r="15" spans="2:12" ht="17.399999999999999">
       <c r="B15" s="35" t="s">
         <v>65</v>
       </c>
@@ -16862,7 +16853,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="18">
+    <row r="16" spans="2:12" ht="17.399999999999999">
       <c r="B16" s="35" t="s">
         <v>26</v>
       </c>
@@ -16891,7 +16882,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="18">
+    <row r="17" spans="2:13" ht="17.399999999999999">
       <c r="B17" s="35" t="s">
         <v>31</v>
       </c>
@@ -16920,7 +16911,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="18">
+    <row r="18" spans="2:13" ht="17.399999999999999">
       <c r="B18" s="35" t="s">
         <v>34</v>
       </c>
@@ -16949,7 +16940,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="18">
+    <row r="19" spans="2:13" ht="17.399999999999999">
       <c r="B19" s="35" t="s">
         <v>36</v>
       </c>
@@ -16978,7 +16969,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="18">
+    <row r="20" spans="2:13" ht="17.399999999999999">
       <c r="B20" s="35" t="s">
         <v>39</v>
       </c>
@@ -17007,7 +16998,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="18">
+    <row r="21" spans="2:13" ht="17.399999999999999">
       <c r="B21" s="35" t="s">
         <v>42</v>
       </c>
@@ -17036,7 +17027,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="18">
+    <row r="22" spans="2:13" ht="17.399999999999999">
       <c r="B22" s="35" t="s">
         <v>44</v>
       </c>
@@ -17065,7 +17056,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="18">
+    <row r="23" spans="2:13" ht="17.399999999999999">
       <c r="B23" s="35" t="s">
         <v>246</v>
       </c>
@@ -17094,7 +17085,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="18">
+    <row r="24" spans="2:13" ht="17.399999999999999">
       <c r="B24" s="35" t="s">
         <v>248</v>
       </c>
@@ -17123,7 +17114,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="18">
+    <row r="25" spans="2:13" ht="17.399999999999999">
       <c r="B25" s="35" t="s">
         <v>754</v>
       </c>
@@ -17152,7 +17143,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="18">
+    <row r="26" spans="2:13" ht="17.399999999999999">
       <c r="B26" s="35" t="s">
         <v>653</v>
       </c>
@@ -17181,7 +17172,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="18">
+    <row r="27" spans="2:13" ht="17.399999999999999">
       <c r="B27" s="35" t="s">
         <v>652</v>
       </c>
@@ -17210,7 +17201,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="18">
+    <row r="28" spans="2:13" ht="17.399999999999999">
       <c r="B28" s="35"/>
       <c r="C28" s="35"/>
       <c r="D28" s="34"/>
@@ -17222,7 +17213,7 @@
       <c r="J28" s="109"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="2:13" ht="18">
+    <row r="29" spans="2:13" ht="17.399999999999999">
       <c r="B29" s="40" t="s">
         <v>8</v>
       </c>
@@ -17251,7 +17242,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="18">
+    <row r="30" spans="2:13" ht="17.399999999999999">
       <c r="B30" s="35" t="s">
         <v>11</v>
       </c>
@@ -17280,7 +17271,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="18">
+    <row r="31" spans="2:13" ht="17.399999999999999">
       <c r="B31" s="35" t="s">
         <v>13</v>
       </c>
@@ -17309,7 +17300,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="32" spans="2:13" s="33" customFormat="1" ht="18">
+    <row r="32" spans="2:13" s="33" customFormat="1" ht="17.399999999999999">
       <c r="B32" s="35" t="s">
         <v>16</v>
       </c>
@@ -17319,7 +17310,7 @@
       </c>
       <c r="E32" s="35"/>
       <c r="F32" s="37" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="G32" s="45">
         <v>2009</v>
@@ -17338,10 +17329,10 @@
         <v>614</v>
       </c>
       <c r="M32" s="84" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" ht="18">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="17.399999999999999">
       <c r="B33" s="35" t="s">
         <v>398</v>
       </c>
@@ -17370,7 +17361,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="18">
+    <row r="34" spans="2:12" ht="17.399999999999999">
       <c r="B34" s="35" t="s">
         <v>485</v>
       </c>
@@ -17399,7 +17390,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="35" spans="2:12" ht="18">
+    <row r="35" spans="2:12" ht="17.399999999999999">
       <c r="B35" s="35" t="s">
         <v>608</v>
       </c>
@@ -17428,7 +17419,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="36" spans="2:12" ht="18">
+    <row r="36" spans="2:12" ht="17.399999999999999">
       <c r="B36" s="35" t="s">
         <v>65</v>
       </c>
@@ -17457,7 +17448,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="18">
+    <row r="37" spans="2:12" ht="17.399999999999999">
       <c r="B37" s="35" t="s">
         <v>26</v>
       </c>
@@ -17486,7 +17477,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="38" spans="2:12" ht="18">
+    <row r="38" spans="2:12" ht="17.399999999999999">
       <c r="B38" s="35" t="s">
         <v>31</v>
       </c>
@@ -17515,7 +17506,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="39" spans="2:12" ht="18">
+    <row r="39" spans="2:12" ht="17.399999999999999">
       <c r="B39" s="35" t="s">
         <v>34</v>
       </c>
@@ -17544,7 +17535,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="18">
+    <row r="40" spans="2:12" ht="17.399999999999999">
       <c r="B40" s="35" t="s">
         <v>36</v>
       </c>
@@ -17573,7 +17564,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="18">
+    <row r="41" spans="2:12" ht="17.399999999999999">
       <c r="B41" s="35" t="s">
         <v>39</v>
       </c>
@@ -17602,7 +17593,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="42" spans="2:12" ht="18">
+    <row r="42" spans="2:12" ht="17.399999999999999">
       <c r="B42" s="40" t="s">
         <v>42</v>
       </c>
@@ -17631,7 +17622,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="43" spans="2:12" ht="18">
+    <row r="43" spans="2:12" ht="17.399999999999999">
       <c r="B43" s="35" t="s">
         <v>44</v>
       </c>
@@ -17660,7 +17651,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="44" spans="2:12" ht="17.45" customHeight="1">
+    <row r="44" spans="2:12" ht="17.399999999999999" customHeight="1">
       <c r="B44" s="40" t="s">
         <v>486</v>
       </c>
@@ -17689,7 +17680,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="45" spans="2:12" ht="17.45" customHeight="1">
+    <row r="45" spans="2:12" ht="17.399999999999999" customHeight="1">
       <c r="B45" s="40" t="s">
         <v>487</v>
       </c>
@@ -17718,7 +17709,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="17.45" customHeight="1">
+    <row r="46" spans="2:12" ht="17.399999999999999" customHeight="1">
       <c r="B46" s="40" t="s">
         <v>754</v>
       </c>
@@ -17747,7 +17738,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="17.45" customHeight="1">
+    <row r="47" spans="2:12" ht="17.399999999999999" customHeight="1">
       <c r="B47" s="35" t="s">
         <v>653</v>
       </c>
@@ -17776,7 +17767,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="48" spans="2:12" ht="17.45" customHeight="1">
+    <row r="48" spans="2:12" ht="17.399999999999999" customHeight="1">
       <c r="B48" s="35" t="s">
         <v>652</v>
       </c>
@@ -17805,7 +17796,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="49" spans="2:13" ht="17.45" customHeight="1">
+    <row r="49" spans="2:13" ht="17.399999999999999" customHeight="1">
       <c r="B49" s="40"/>
       <c r="C49" s="40"/>
       <c r="D49" s="34"/>
@@ -17817,7 +17808,7 @@
       <c r="J49" s="109"/>
       <c r="K49" s="9"/>
     </row>
-    <row r="50" spans="2:13" ht="17.45" customHeight="1">
+    <row r="50" spans="2:13" ht="17.399999999999999" customHeight="1">
       <c r="B50" s="40" t="s">
         <v>8</v>
       </c>
@@ -17846,7 +17837,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="51" spans="2:13" ht="17.45" customHeight="1">
+    <row r="51" spans="2:13" ht="17.399999999999999" customHeight="1">
       <c r="B51" s="35" t="s">
         <v>11</v>
       </c>
@@ -17875,7 +17866,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="52" spans="2:13" ht="17.45" customHeight="1">
+    <row r="52" spans="2:13" ht="17.399999999999999" customHeight="1">
       <c r="B52" s="35" t="s">
         <v>264</v>
       </c>
@@ -17904,7 +17895,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="53" spans="2:13" ht="18">
+    <row r="53" spans="2:13" ht="17.399999999999999">
       <c r="B53" s="35" t="s">
         <v>13</v>
       </c>
@@ -17933,7 +17924,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="54" spans="2:13" ht="18">
+    <row r="54" spans="2:13" ht="17.399999999999999">
       <c r="B54" s="35" t="s">
         <v>16</v>
       </c>
@@ -17962,7 +17953,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="55" spans="2:13" ht="18">
+    <row r="55" spans="2:13" ht="17.399999999999999">
       <c r="B55" s="35" t="s">
         <v>398</v>
       </c>
@@ -17991,7 +17982,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="56" spans="2:13" ht="18">
+    <row r="56" spans="2:13" ht="17.399999999999999">
       <c r="B56" s="35" t="s">
         <v>485</v>
       </c>
@@ -18020,7 +18011,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="57" spans="2:13" ht="18">
+    <row r="57" spans="2:13" ht="17.399999999999999">
       <c r="B57" s="35" t="s">
         <v>65</v>
       </c>
@@ -18040,7 +18031,7 @@
         <v>251</v>
       </c>
       <c r="J57" s="117" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="K57" s="84" t="s">
         <v>870</v>
@@ -18049,7 +18040,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="58" spans="2:13" ht="18">
+    <row r="58" spans="2:13" ht="17.399999999999999">
       <c r="B58" s="35" t="s">
         <v>65</v>
       </c>
@@ -18069,7 +18060,7 @@
         <v>488</v>
       </c>
       <c r="J58" s="117" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="K58" s="84" t="s">
         <v>870</v>
@@ -18081,7 +18072,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="59" spans="2:13" ht="18">
+    <row r="59" spans="2:13" ht="17.399999999999999">
       <c r="B59" s="35" t="s">
         <v>268</v>
       </c>
@@ -18113,7 +18104,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="60" spans="2:13" ht="18">
+    <row r="60" spans="2:13" ht="17.399999999999999">
       <c r="B60" s="35" t="s">
         <v>26</v>
       </c>
@@ -18145,7 +18136,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="61" spans="2:13" ht="18">
+    <row r="61" spans="2:13" ht="17.399999999999999">
       <c r="B61" s="35" t="s">
         <v>31</v>
       </c>
@@ -18174,7 +18165,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="62" spans="2:13" ht="18">
+    <row r="62" spans="2:13" ht="17.399999999999999">
       <c r="B62" s="35" t="s">
         <v>34</v>
       </c>
@@ -18203,7 +18194,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="63" spans="2:13" ht="18">
+    <row r="63" spans="2:13" ht="17.399999999999999">
       <c r="B63" s="35" t="s">
         <v>36</v>
       </c>
@@ -18232,7 +18223,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="64" spans="2:13" ht="18">
+    <row r="64" spans="2:13" ht="17.399999999999999">
       <c r="B64" s="35" t="s">
         <v>39</v>
       </c>
@@ -18261,7 +18252,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="65" spans="2:13" ht="18">
+    <row r="65" spans="2:13" ht="17.399999999999999">
       <c r="B65" s="35" t="s">
         <v>42</v>
       </c>
@@ -18293,7 +18284,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="66" spans="2:13" ht="18">
+    <row r="66" spans="2:13" ht="17.399999999999999">
       <c r="B66" s="35" t="s">
         <v>44</v>
       </c>
@@ -18322,7 +18313,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="67" spans="2:13" ht="17.45" customHeight="1">
+    <row r="67" spans="2:13" ht="17.399999999999999" customHeight="1">
       <c r="B67" s="35" t="s">
         <v>277</v>
       </c>
@@ -18354,7 +18345,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="68" spans="2:13" ht="18">
+    <row r="68" spans="2:13" ht="17.399999999999999">
       <c r="B68" s="35" t="s">
         <v>278</v>
       </c>
@@ -18374,7 +18365,7 @@
         <v>280</v>
       </c>
       <c r="J68" s="112" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="K68" s="84" t="s">
         <v>870</v>
@@ -18383,10 +18374,10 @@
         <v>838</v>
       </c>
       <c r="M68" s="84" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="69" spans="2:13" ht="18">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13" ht="17.399999999999999">
       <c r="B69" s="35" t="s">
         <v>754</v>
       </c>
@@ -18418,7 +18409,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="70" spans="2:13" ht="18">
+    <row r="70" spans="2:13" ht="17.399999999999999">
       <c r="B70" s="40" t="s">
         <v>781</v>
       </c>
@@ -18438,7 +18429,7 @@
         <v>282</v>
       </c>
       <c r="J70" s="112" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="K70" s="84" t="s">
         <v>870</v>
@@ -18447,10 +18438,10 @@
         <v>838</v>
       </c>
       <c r="M70" s="84" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="71" spans="2:13" ht="18">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" ht="17.399999999999999">
       <c r="B71" s="35" t="s">
         <v>653</v>
       </c>
@@ -18479,7 +18470,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="72" spans="2:13" ht="18">
+    <row r="72" spans="2:13" ht="17.399999999999999">
       <c r="B72" s="35" t="s">
         <v>652</v>
       </c>
@@ -18508,7 +18499,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="74" spans="2:13" ht="18">
+    <row r="74" spans="2:13" ht="17.399999999999999">
       <c r="B74" s="35" t="s">
         <v>8</v>
       </c>
@@ -18537,7 +18528,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="75" spans="2:13" ht="18">
+    <row r="75" spans="2:13" ht="17.399999999999999">
       <c r="B75" s="35" t="s">
         <v>11</v>
       </c>
@@ -18566,7 +18557,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="76" spans="2:13" ht="18">
+    <row r="76" spans="2:13" ht="17.399999999999999">
       <c r="B76" s="35" t="s">
         <v>264</v>
       </c>
@@ -18595,7 +18586,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="77" spans="2:13" ht="18">
+    <row r="77" spans="2:13" ht="17.399999999999999">
       <c r="B77" s="35" t="s">
         <v>16</v>
       </c>
@@ -18624,7 +18615,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="78" spans="2:13" ht="18">
+    <row r="78" spans="2:13" ht="17.399999999999999">
       <c r="B78" s="35" t="s">
         <v>398</v>
       </c>
@@ -18653,7 +18644,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="79" spans="2:13" ht="18">
+    <row r="79" spans="2:13" ht="17.399999999999999">
       <c r="B79" s="35" t="s">
         <v>485</v>
       </c>
@@ -18682,7 +18673,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="80" spans="2:13" ht="18">
+    <row r="80" spans="2:13" ht="17.399999999999999">
       <c r="B80" s="35" t="s">
         <v>65</v>
       </c>
@@ -18711,7 +18702,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="81" spans="2:13" ht="18">
+    <row r="81" spans="2:13" ht="17.399999999999999">
       <c r="B81" s="35" t="s">
         <v>31</v>
       </c>
@@ -18740,7 +18731,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="82" spans="2:13" ht="18">
+    <row r="82" spans="2:13" ht="17.399999999999999">
       <c r="B82" s="35" t="s">
         <v>34</v>
       </c>
@@ -18769,7 +18760,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="83" spans="2:13" ht="18">
+    <row r="83" spans="2:13" ht="17.399999999999999">
       <c r="B83" s="35" t="s">
         <v>36</v>
       </c>
@@ -18798,7 +18789,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="84" spans="2:13" ht="18">
+    <row r="84" spans="2:13" ht="17.399999999999999">
       <c r="B84" s="35" t="s">
         <v>42</v>
       </c>
@@ -18830,7 +18821,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="85" spans="2:13" ht="18">
+    <row r="85" spans="2:13" ht="17.399999999999999">
       <c r="B85" s="35" t="s">
         <v>44</v>
       </c>
@@ -18862,7 +18853,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="86" spans="2:13" ht="18">
+    <row r="86" spans="2:13" ht="17.399999999999999">
       <c r="B86" s="35" t="s">
         <v>277</v>
       </c>
@@ -18891,10 +18882,10 @@
         <v>845</v>
       </c>
       <c r="M86" s="84" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="87" spans="2:13" ht="18">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="87" spans="2:13" ht="17.399999999999999">
       <c r="B87" s="35" t="s">
         <v>278</v>
       </c>
@@ -18914,7 +18905,7 @@
         <v>296</v>
       </c>
       <c r="J87" s="112" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="K87" s="84" t="s">
         <v>870</v>
@@ -18923,10 +18914,10 @@
         <v>845</v>
       </c>
       <c r="M87" s="84" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="88" spans="2:13" ht="18">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="88" spans="2:13" ht="17.399999999999999">
       <c r="B88" s="35" t="s">
         <v>754</v>
       </c>
@@ -18958,7 +18949,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="89" spans="2:13" ht="18">
+    <row r="89" spans="2:13" ht="17.399999999999999">
       <c r="B89" s="35" t="s">
         <v>520</v>
       </c>
@@ -18978,7 +18969,7 @@
         <v>282</v>
       </c>
       <c r="J89" s="112" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="K89" s="84" t="s">
         <v>870</v>
@@ -18987,10 +18978,10 @@
         <v>845</v>
       </c>
       <c r="M89" s="84" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="90" spans="2:13" ht="18">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="90" spans="2:13" ht="17.399999999999999">
       <c r="B90" s="35" t="s">
         <v>653</v>
       </c>
@@ -19019,7 +19010,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="91" spans="2:13" ht="18">
+    <row r="91" spans="2:13" ht="17.399999999999999">
       <c r="B91" s="35"/>
       <c r="C91" s="35"/>
       <c r="D91" s="34"/>
@@ -19031,7 +19022,7 @@
       <c r="J91" s="112"/>
       <c r="K91" s="9"/>
     </row>
-    <row r="92" spans="2:13" ht="18">
+    <row r="92" spans="2:13" ht="17.399999999999999">
       <c r="B92" s="35" t="s">
         <v>8</v>
       </c>
@@ -19060,7 +19051,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="93" spans="2:13" ht="18">
+    <row r="93" spans="2:13" ht="17.399999999999999">
       <c r="B93" s="35" t="s">
         <v>11</v>
       </c>
@@ -19089,7 +19080,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="94" spans="2:13" ht="18">
+    <row r="94" spans="2:13" ht="17.399999999999999">
       <c r="B94" s="35" t="s">
         <v>16</v>
       </c>
@@ -19118,7 +19109,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="95" spans="2:13" ht="18">
+    <row r="95" spans="2:13" ht="17.399999999999999">
       <c r="B95" s="35" t="s">
         <v>398</v>
       </c>
@@ -19147,7 +19138,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="96" spans="2:13" ht="18">
+    <row r="96" spans="2:13" ht="17.399999999999999">
       <c r="B96" s="35" t="s">
         <v>485</v>
       </c>
@@ -19176,7 +19167,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="97" spans="2:13" ht="18">
+    <row r="97" spans="2:13" ht="17.399999999999999">
       <c r="B97" s="35" t="s">
         <v>304</v>
       </c>
@@ -19208,7 +19199,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="98" spans="2:13" ht="18">
+    <row r="98" spans="2:13" ht="17.399999999999999">
       <c r="B98" s="35" t="s">
         <v>305</v>
       </c>
@@ -19240,7 +19231,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="99" spans="2:13" ht="18">
+    <row r="99" spans="2:13" ht="17.399999999999999">
       <c r="B99" s="35" t="s">
         <v>31</v>
       </c>
@@ -19269,7 +19260,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="100" spans="2:13" ht="18">
+    <row r="100" spans="2:13" ht="17.399999999999999">
       <c r="B100" s="35" t="s">
         <v>34</v>
       </c>
@@ -19298,7 +19289,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="101" spans="2:13" ht="18">
+    <row r="101" spans="2:13" ht="17.399999999999999">
       <c r="B101" s="35" t="s">
         <v>307</v>
       </c>
@@ -19327,7 +19318,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="102" spans="2:13" ht="18">
+    <row r="102" spans="2:13" ht="17.399999999999999">
       <c r="B102" s="35" t="s">
         <v>310</v>
       </c>
@@ -19356,7 +19347,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="103" spans="2:13" ht="18">
+    <row r="103" spans="2:13" ht="17.399999999999999">
       <c r="B103" s="35" t="s">
         <v>311</v>
       </c>
@@ -19385,7 +19376,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="104" spans="2:13" ht="18">
+    <row r="104" spans="2:13" ht="17.399999999999999">
       <c r="B104" s="35" t="s">
         <v>313</v>
       </c>
@@ -19414,7 +19405,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="105" spans="2:13" ht="18">
+    <row r="105" spans="2:13" ht="17.399999999999999">
       <c r="B105" s="35" t="s">
         <v>314</v>
       </c>
@@ -19443,7 +19434,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="106" spans="2:13" ht="18">
+    <row r="106" spans="2:13" ht="17.399999999999999">
       <c r="B106" s="35" t="s">
         <v>316</v>
       </c>
@@ -19472,7 +19463,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="107" spans="2:13" ht="18">
+    <row r="107" spans="2:13" ht="17.399999999999999">
       <c r="B107" s="35" t="s">
         <v>709</v>
       </c>
@@ -19501,7 +19492,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="108" spans="2:13" ht="18">
+    <row r="108" spans="2:13" ht="17.399999999999999">
       <c r="B108" s="35" t="s">
         <v>653</v>
       </c>
@@ -19530,7 +19521,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="109" spans="2:13" ht="18">
+    <row r="109" spans="2:13" ht="17.399999999999999">
       <c r="B109" s="35"/>
       <c r="C109" s="35"/>
       <c r="D109" s="34"/>
@@ -19541,7 +19532,7 @@
       <c r="I109" s="37"/>
       <c r="J109" s="109"/>
     </row>
-    <row r="110" spans="2:13" ht="18">
+    <row r="110" spans="2:13" ht="17.399999999999999">
       <c r="B110" s="40" t="s">
         <v>534</v>
       </c>
@@ -19570,7 +19561,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="111" spans="2:13" ht="18">
+    <row r="111" spans="2:13" ht="17.399999999999999">
       <c r="B111" s="40" t="s">
         <v>510</v>
       </c>
@@ -19599,7 +19590,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="112" spans="2:13" ht="18">
+    <row r="112" spans="2:13" ht="17.399999999999999">
       <c r="B112" s="35" t="s">
         <v>34</v>
       </c>
@@ -19649,7 +19640,7 @@
       <c r="H114" s="15"/>
       <c r="I114" s="14"/>
     </row>
-    <row r="115" spans="2:10" ht="19.5">
+    <row r="115" spans="2:10" ht="20.399999999999999">
       <c r="B115" s="91"/>
       <c r="C115" s="13"/>
       <c r="D115" s="15"/>
@@ -19659,7 +19650,7 @@
       <c r="H115" s="15"/>
       <c r="I115" s="96"/>
     </row>
-    <row r="116" spans="2:10" ht="19.5">
+    <row r="116" spans="2:10" ht="20.399999999999999">
       <c r="B116" s="91"/>
       <c r="C116" s="13"/>
       <c r="D116" s="15"/>
@@ -19669,7 +19660,7 @@
       <c r="H116" s="15"/>
       <c r="I116" s="14"/>
     </row>
-    <row r="117" spans="2:10" ht="17.45" customHeight="1">
+    <row r="117" spans="2:10" ht="17.399999999999999" customHeight="1">
       <c r="B117" s="35"/>
       <c r="C117" s="91"/>
       <c r="D117" s="35"/>
@@ -19689,7 +19680,7 @@
       <c r="H118" s="15"/>
       <c r="I118" s="14"/>
     </row>
-    <row r="119" spans="2:10" ht="18">
+    <row r="119" spans="2:10" ht="17.399999999999999">
       <c r="B119" s="35"/>
       <c r="C119" s="35"/>
       <c r="D119" s="35"/>
@@ -19699,7 +19690,7 @@
       <c r="H119" s="35"/>
       <c r="I119" s="35"/>
     </row>
-    <row r="120" spans="2:10" ht="18">
+    <row r="120" spans="2:10" ht="17.399999999999999">
       <c r="B120" s="35"/>
       <c r="C120" s="35"/>
       <c r="D120" s="35"/>
@@ -19709,7 +19700,7 @@
       <c r="H120" s="35"/>
       <c r="I120" s="35"/>
     </row>
-    <row r="121" spans="2:10" ht="18">
+    <row r="121" spans="2:10" ht="17.399999999999999">
       <c r="B121" s="35"/>
       <c r="C121" s="35"/>
       <c r="D121" s="35"/>
@@ -19719,7 +19710,7 @@
       <c r="H121" s="35"/>
       <c r="I121" s="35"/>
     </row>
-    <row r="122" spans="2:10" ht="18">
+    <row r="122" spans="2:10" ht="17.399999999999999">
       <c r="B122" s="35"/>
       <c r="C122" s="35"/>
       <c r="D122" s="35"/>
@@ -19729,7 +19720,7 @@
       <c r="H122" s="35"/>
       <c r="I122" s="35"/>
     </row>
-    <row r="123" spans="2:10" ht="18">
+    <row r="123" spans="2:10" ht="17.399999999999999">
       <c r="B123" s="35"/>
       <c r="C123" s="35"/>
       <c r="D123" s="35"/>
@@ -19739,7 +19730,7 @@
       <c r="H123" s="35"/>
       <c r="I123" s="35"/>
     </row>
-    <row r="124" spans="2:10" ht="18">
+    <row r="124" spans="2:10" ht="17.399999999999999">
       <c r="B124" s="35"/>
       <c r="C124" s="35"/>
       <c r="D124" s="34"/>
@@ -19749,7 +19740,7 @@
       <c r="H124" s="34"/>
       <c r="I124" s="35"/>
     </row>
-    <row r="125" spans="2:10" ht="18">
+    <row r="125" spans="2:10" ht="17.399999999999999">
       <c r="B125" s="35"/>
       <c r="C125" s="35"/>
       <c r="D125" s="35"/>
@@ -19759,7 +19750,7 @@
       <c r="H125" s="35"/>
       <c r="I125" s="35"/>
     </row>
-    <row r="126" spans="2:10" ht="18">
+    <row r="126" spans="2:10" ht="17.399999999999999">
       <c r="B126" s="35"/>
       <c r="C126" s="35"/>
       <c r="D126" s="35"/>
@@ -19769,7 +19760,7 @@
       <c r="H126" s="35"/>
       <c r="I126" s="35"/>
     </row>
-    <row r="127" spans="2:10" ht="18">
+    <row r="127" spans="2:10" ht="17.399999999999999">
       <c r="B127" s="35"/>
       <c r="C127" s="35"/>
       <c r="D127" s="35"/>
@@ -19779,7 +19770,7 @@
       <c r="H127" s="35"/>
       <c r="I127" s="35"/>
     </row>
-    <row r="128" spans="2:10" ht="18">
+    <row r="128" spans="2:10" ht="17.399999999999999">
       <c r="B128" s="35"/>
       <c r="C128" s="35"/>
       <c r="D128" s="35"/>
@@ -19789,7 +19780,7 @@
       <c r="H128" s="35"/>
       <c r="I128" s="35"/>
     </row>
-    <row r="129" spans="2:9" ht="18">
+    <row r="129" spans="2:9" ht="17.399999999999999">
       <c r="B129" s="35"/>
       <c r="C129" s="35"/>
       <c r="D129" s="35"/>
@@ -19799,7 +19790,7 @@
       <c r="H129" s="35"/>
       <c r="I129" s="35"/>
     </row>
-    <row r="130" spans="2:9" ht="18">
+    <row r="130" spans="2:9" ht="17.399999999999999">
       <c r="B130" s="35"/>
       <c r="C130" s="35"/>
       <c r="D130" s="34"/>
@@ -19809,7 +19800,7 @@
       <c r="H130" s="34"/>
       <c r="I130" s="35"/>
     </row>
-    <row r="131" spans="2:9" ht="18">
+    <row r="131" spans="2:9" ht="17.399999999999999">
       <c r="B131" s="35"/>
       <c r="C131" s="35"/>
       <c r="D131" s="35"/>
@@ -19819,7 +19810,7 @@
       <c r="H131" s="35"/>
       <c r="I131" s="35"/>
     </row>
-    <row r="132" spans="2:9" ht="18">
+    <row r="132" spans="2:9" ht="17.399999999999999">
       <c r="B132" s="35"/>
       <c r="C132" s="35"/>
       <c r="D132" s="35"/>
@@ -19829,7 +19820,7 @@
       <c r="H132" s="35"/>
       <c r="I132" s="35"/>
     </row>
-    <row r="133" spans="2:9" ht="18">
+    <row r="133" spans="2:9" ht="17.399999999999999">
       <c r="B133" s="35"/>
       <c r="C133" s="35"/>
       <c r="D133" s="34"/>
@@ -19839,7 +19830,7 @@
       <c r="H133" s="34"/>
       <c r="I133" s="35"/>
     </row>
-    <row r="134" spans="2:9" ht="18">
+    <row r="134" spans="2:9" ht="17.399999999999999">
       <c r="B134" s="35"/>
       <c r="C134" s="35"/>
       <c r="D134" s="35"/>
@@ -19849,7 +19840,7 @@
       <c r="H134" s="35"/>
       <c r="I134" s="35"/>
     </row>
-    <row r="135" spans="2:9" ht="18">
+    <row r="135" spans="2:9" ht="17.399999999999999">
       <c r="B135" s="35"/>
       <c r="C135" s="35"/>
       <c r="D135" s="35"/>
@@ -19859,7 +19850,7 @@
       <c r="H135" s="35"/>
       <c r="I135" s="35"/>
     </row>
-    <row r="136" spans="2:9" ht="18">
+    <row r="136" spans="2:9" ht="17.399999999999999">
       <c r="B136" s="35"/>
       <c r="C136" s="35"/>
       <c r="D136" s="35"/>
@@ -19869,7 +19860,7 @@
       <c r="H136" s="35"/>
       <c r="I136" s="35"/>
     </row>
-    <row r="137" spans="2:9" ht="18">
+    <row r="137" spans="2:9" ht="17.399999999999999">
       <c r="B137" s="35"/>
       <c r="C137" s="35"/>
       <c r="D137" s="35"/>
@@ -19879,7 +19870,7 @@
       <c r="H137" s="35"/>
       <c r="I137" s="35"/>
     </row>
-    <row r="138" spans="2:9" ht="18">
+    <row r="138" spans="2:9" ht="17.399999999999999">
       <c r="B138" s="35"/>
       <c r="C138" s="35"/>
       <c r="D138" s="35"/>
@@ -19889,7 +19880,7 @@
       <c r="H138" s="35"/>
       <c r="I138" s="35"/>
     </row>
-    <row r="139" spans="2:9" ht="18">
+    <row r="139" spans="2:9" ht="17.399999999999999">
       <c r="B139" s="35"/>
       <c r="C139" s="35"/>
       <c r="D139" s="34"/>
@@ -19899,7 +19890,7 @@
       <c r="H139" s="34"/>
       <c r="I139" s="35"/>
     </row>
-    <row r="140" spans="2:9" ht="18">
+    <row r="140" spans="2:9" ht="17.399999999999999">
       <c r="B140" s="35"/>
       <c r="C140" s="35"/>
       <c r="D140" s="35"/>
@@ -19909,7 +19900,7 @@
       <c r="H140" s="35"/>
       <c r="I140" s="35"/>
     </row>
-    <row r="141" spans="2:9" ht="18">
+    <row r="141" spans="2:9" ht="17.399999999999999">
       <c r="B141" s="35"/>
       <c r="C141" s="35"/>
       <c r="D141" s="35"/>
@@ -19919,7 +19910,7 @@
       <c r="H141" s="35"/>
       <c r="I141" s="35"/>
     </row>
-    <row r="142" spans="2:9" ht="18">
+    <row r="142" spans="2:9" ht="17.399999999999999">
       <c r="B142" s="35"/>
       <c r="C142" s="35"/>
       <c r="D142" s="35"/>
@@ -19929,7 +19920,7 @@
       <c r="H142" s="35"/>
       <c r="I142" s="35"/>
     </row>
-    <row r="143" spans="2:9" ht="18">
+    <row r="143" spans="2:9" ht="17.399999999999999">
       <c r="B143" s="35"/>
       <c r="C143" s="35"/>
       <c r="D143" s="35"/>
@@ -19939,7 +19930,7 @@
       <c r="H143" s="35"/>
       <c r="I143" s="35"/>
     </row>
-    <row r="144" spans="2:9" ht="18">
+    <row r="144" spans="2:9" ht="17.399999999999999">
       <c r="B144" s="35"/>
       <c r="C144" s="35"/>
       <c r="D144" s="35"/>
@@ -19949,7 +19940,7 @@
       <c r="H144" s="35"/>
       <c r="I144" s="35"/>
     </row>
-    <row r="145" spans="2:9" ht="18">
+    <row r="145" spans="2:9" ht="17.399999999999999">
       <c r="B145" s="35"/>
       <c r="C145" s="35"/>
       <c r="D145" s="34"/>
@@ -19959,7 +19950,7 @@
       <c r="H145" s="34"/>
       <c r="I145" s="37"/>
     </row>
-    <row r="146" spans="2:9" ht="18">
+    <row r="146" spans="2:9" ht="17.399999999999999">
       <c r="B146" s="35"/>
       <c r="C146" s="35"/>
       <c r="D146" s="35"/>
@@ -19969,7 +19960,7 @@
       <c r="H146" s="35"/>
       <c r="I146" s="35"/>
     </row>
-    <row r="147" spans="2:9" ht="18">
+    <row r="147" spans="2:9" ht="17.399999999999999">
       <c r="B147" s="35"/>
       <c r="C147" s="35"/>
       <c r="D147" s="35"/>
@@ -19979,7 +19970,7 @@
       <c r="H147" s="35"/>
       <c r="I147" s="35"/>
     </row>
-    <row r="148" spans="2:9" ht="18">
+    <row r="148" spans="2:9" ht="17.399999999999999">
       <c r="B148" s="35"/>
       <c r="C148" s="35"/>
       <c r="D148" s="35"/>
@@ -19989,7 +19980,7 @@
       <c r="H148" s="35"/>
       <c r="I148" s="35"/>
     </row>
-    <row r="149" spans="2:9" ht="18">
+    <row r="149" spans="2:9" ht="17.399999999999999">
       <c r="B149" s="35"/>
       <c r="C149" s="35"/>
       <c r="D149" s="35"/>
@@ -19999,7 +19990,7 @@
       <c r="H149" s="35"/>
       <c r="I149" s="35"/>
     </row>
-    <row r="150" spans="2:9" ht="18">
+    <row r="150" spans="2:9" ht="17.399999999999999">
       <c r="B150" s="35"/>
       <c r="C150" s="35"/>
       <c r="D150" s="35"/>
@@ -20009,7 +20000,7 @@
       <c r="H150" s="35"/>
       <c r="I150" s="35"/>
     </row>
-    <row r="151" spans="2:9" ht="18">
+    <row r="151" spans="2:9" ht="17.399999999999999">
       <c r="B151" s="35"/>
       <c r="C151" s="35"/>
       <c r="D151" s="35"/>
@@ -20019,7 +20010,7 @@
       <c r="H151" s="35"/>
       <c r="I151" s="35"/>
     </row>
-    <row r="152" spans="2:9" ht="18">
+    <row r="152" spans="2:9" ht="17.399999999999999">
       <c r="B152" s="35"/>
       <c r="C152" s="35"/>
       <c r="D152" s="35"/>
@@ -20029,7 +20020,7 @@
       <c r="H152" s="35"/>
       <c r="I152" s="35"/>
     </row>
-    <row r="153" spans="2:9" ht="18">
+    <row r="153" spans="2:9" ht="17.399999999999999">
       <c r="B153" s="35"/>
       <c r="C153" s="35"/>
       <c r="D153" s="35"/>
@@ -20039,7 +20030,7 @@
       <c r="H153" s="35"/>
       <c r="I153" s="35"/>
     </row>
-    <row r="154" spans="2:9" ht="18">
+    <row r="154" spans="2:9" ht="17.399999999999999">
       <c r="B154" s="35"/>
       <c r="C154" s="35"/>
       <c r="D154" s="35"/>
@@ -20049,7 +20040,7 @@
       <c r="H154" s="35"/>
       <c r="I154" s="35"/>
     </row>
-    <row r="155" spans="2:9" ht="18">
+    <row r="155" spans="2:9" ht="17.399999999999999">
       <c r="B155" s="35"/>
       <c r="C155" s="35"/>
       <c r="D155" s="35"/>
@@ -20059,7 +20050,7 @@
       <c r="H155" s="35"/>
       <c r="I155" s="35"/>
     </row>
-    <row r="156" spans="2:9" ht="18">
+    <row r="156" spans="2:9" ht="17.399999999999999">
       <c r="B156" s="35"/>
       <c r="C156" s="35"/>
       <c r="D156" s="35"/>
@@ -20069,7 +20060,7 @@
       <c r="H156" s="35"/>
       <c r="I156" s="35"/>
     </row>
-    <row r="157" spans="2:9" ht="18">
+    <row r="157" spans="2:9" ht="17.399999999999999">
       <c r="B157" s="35"/>
       <c r="C157" s="35"/>
       <c r="D157" s="35"/>
@@ -20079,7 +20070,7 @@
       <c r="H157" s="35"/>
       <c r="I157" s="35"/>
     </row>
-    <row r="158" spans="2:9" ht="18">
+    <row r="158" spans="2:9" ht="17.399999999999999">
       <c r="B158" s="35"/>
       <c r="C158" s="35"/>
       <c r="D158" s="35"/>
@@ -20089,7 +20080,7 @@
       <c r="H158" s="35"/>
       <c r="I158" s="35"/>
     </row>
-    <row r="159" spans="2:9" ht="18">
+    <row r="159" spans="2:9" ht="17.399999999999999">
       <c r="B159" s="35"/>
       <c r="C159" s="35"/>
       <c r="D159" s="34"/>
@@ -20099,7 +20090,7 @@
       <c r="H159" s="34"/>
       <c r="I159" s="37"/>
     </row>
-    <row r="160" spans="2:9" ht="18">
+    <row r="160" spans="2:9" ht="17.399999999999999">
       <c r="B160" s="35"/>
       <c r="C160" s="35"/>
       <c r="D160" s="35"/>
@@ -20109,7 +20100,7 @@
       <c r="H160" s="35"/>
       <c r="I160" s="35"/>
     </row>
-    <row r="161" spans="2:9" ht="18">
+    <row r="161" spans="2:9" ht="17.399999999999999">
       <c r="B161" s="35"/>
       <c r="C161" s="35"/>
       <c r="D161" s="35"/>
@@ -20119,7 +20110,7 @@
       <c r="H161" s="35"/>
       <c r="I161" s="35"/>
     </row>
-    <row r="162" spans="2:9" ht="18">
+    <row r="162" spans="2:9" ht="17.399999999999999">
       <c r="B162" s="35"/>
       <c r="C162" s="35"/>
       <c r="D162" s="35"/>
@@ -20129,7 +20120,7 @@
       <c r="H162" s="35"/>
       <c r="I162" s="94"/>
     </row>
-    <row r="163" spans="2:9" ht="18">
+    <row r="163" spans="2:9" ht="17.399999999999999">
       <c r="B163" s="35"/>
       <c r="C163" s="35"/>
       <c r="D163" s="35"/>
@@ -20139,7 +20130,7 @@
       <c r="H163" s="35"/>
       <c r="I163" s="95"/>
     </row>
-    <row r="164" spans="2:9" ht="18">
+    <row r="164" spans="2:9" ht="17.399999999999999">
       <c r="B164" s="35"/>
       <c r="C164" s="35"/>
       <c r="D164" s="35"/>
@@ -20149,7 +20140,7 @@
       <c r="H164" s="35"/>
       <c r="I164" s="35"/>
     </row>
-    <row r="165" spans="2:9" ht="18">
+    <row r="165" spans="2:9" ht="17.399999999999999">
       <c r="B165" s="35"/>
       <c r="C165" s="35"/>
       <c r="D165" s="35"/>
@@ -20159,7 +20150,7 @@
       <c r="H165" s="35"/>
       <c r="I165" s="35"/>
     </row>
-    <row r="166" spans="2:9" ht="18">
+    <row r="166" spans="2:9" ht="17.399999999999999">
       <c r="B166" s="35"/>
       <c r="C166" s="35"/>
       <c r="D166" s="35"/>
@@ -20169,7 +20160,7 @@
       <c r="H166" s="35"/>
       <c r="I166" s="35"/>
     </row>
-    <row r="167" spans="2:9" ht="18">
+    <row r="167" spans="2:9" ht="17.399999999999999">
       <c r="B167" s="35"/>
       <c r="C167" s="35"/>
       <c r="D167" s="34"/>
@@ -20179,7 +20170,7 @@
       <c r="H167" s="34"/>
       <c r="I167" s="35"/>
     </row>
-    <row r="168" spans="2:9" ht="18">
+    <row r="168" spans="2:9" ht="17.399999999999999">
       <c r="B168" s="35"/>
       <c r="C168" s="35"/>
       <c r="D168" s="35"/>
@@ -20189,7 +20180,7 @@
       <c r="H168" s="35"/>
       <c r="I168" s="35"/>
     </row>
-    <row r="169" spans="2:9" ht="18">
+    <row r="169" spans="2:9" ht="17.399999999999999">
       <c r="B169" s="35"/>
       <c r="C169" s="35"/>
       <c r="D169" s="34"/>
@@ -20199,7 +20190,7 @@
       <c r="H169" s="34"/>
       <c r="I169" s="35"/>
     </row>
-    <row r="170" spans="2:9" ht="18">
+    <row r="170" spans="2:9" ht="17.399999999999999">
       <c r="B170" s="35"/>
       <c r="C170" s="35"/>
       <c r="D170" s="35"/>
@@ -20209,7 +20200,7 @@
       <c r="H170" s="35"/>
       <c r="I170" s="35"/>
     </row>
-    <row r="171" spans="2:9" ht="18">
+    <row r="171" spans="2:9" ht="17.399999999999999">
       <c r="B171" s="35"/>
       <c r="C171" s="35"/>
       <c r="D171" s="35"/>
@@ -20219,7 +20210,7 @@
       <c r="H171" s="35"/>
       <c r="I171" s="35"/>
     </row>
-    <row r="172" spans="2:9" ht="18">
+    <row r="172" spans="2:9" ht="17.399999999999999">
       <c r="B172" s="35"/>
       <c r="C172" s="35"/>
       <c r="D172" s="35"/>
@@ -20229,7 +20220,7 @@
       <c r="H172" s="35"/>
       <c r="I172" s="35"/>
     </row>
-    <row r="173" spans="2:9" ht="18">
+    <row r="173" spans="2:9" ht="17.399999999999999">
       <c r="B173" s="35"/>
       <c r="C173" s="35"/>
       <c r="D173" s="34"/>
@@ -20239,7 +20230,7 @@
       <c r="H173" s="34"/>
       <c r="I173" s="35"/>
     </row>
-    <row r="174" spans="2:9" ht="18">
+    <row r="174" spans="2:9" ht="17.399999999999999">
       <c r="B174" s="35"/>
       <c r="C174" s="35"/>
       <c r="D174" s="35"/>
@@ -20249,7 +20240,7 @@
       <c r="H174" s="35"/>
       <c r="I174" s="35"/>
     </row>
-    <row r="175" spans="2:9" ht="18">
+    <row r="175" spans="2:9" ht="17.399999999999999">
       <c r="B175" s="35"/>
       <c r="C175" s="35"/>
       <c r="D175" s="35"/>
@@ -20259,7 +20250,7 @@
       <c r="H175" s="35"/>
       <c r="I175" s="35"/>
     </row>
-    <row r="176" spans="2:9" ht="18">
+    <row r="176" spans="2:9" ht="17.399999999999999">
       <c r="B176" s="35"/>
       <c r="C176" s="35"/>
       <c r="D176" s="35"/>
@@ -20269,7 +20260,7 @@
       <c r="H176" s="35"/>
       <c r="I176" s="35"/>
     </row>
-    <row r="177" spans="2:10" ht="18">
+    <row r="177" spans="2:10" ht="17.399999999999999">
       <c r="B177" s="35"/>
       <c r="C177" s="35"/>
       <c r="D177" s="35"/>
@@ -20279,7 +20270,7 @@
       <c r="H177" s="35"/>
       <c r="I177" s="35"/>
     </row>
-    <row r="178" spans="2:10" ht="18">
+    <row r="178" spans="2:10" ht="17.399999999999999">
       <c r="B178" s="35"/>
       <c r="C178" s="35"/>
       <c r="D178" s="35"/>
@@ -20289,7 +20280,7 @@
       <c r="H178" s="35"/>
       <c r="I178" s="35"/>
     </row>
-    <row r="179" spans="2:10" ht="18">
+    <row r="179" spans="2:10" ht="17.399999999999999">
       <c r="B179" s="35"/>
       <c r="C179" s="35"/>
       <c r="D179" s="35"/>
@@ -20299,7 +20290,7 @@
       <c r="H179" s="34"/>
       <c r="I179" s="35"/>
     </row>
-    <row r="180" spans="2:10" ht="18">
+    <row r="180" spans="2:10" ht="17.399999999999999">
       <c r="B180" s="35"/>
       <c r="C180" s="35"/>
       <c r="D180" s="35"/>
@@ -20309,7 +20300,7 @@
       <c r="H180" s="35"/>
       <c r="I180" s="35"/>
     </row>
-    <row r="181" spans="2:10" ht="18">
+    <row r="181" spans="2:10" ht="17.399999999999999">
       <c r="B181" s="35"/>
       <c r="C181" s="35"/>
       <c r="D181" s="35"/>
@@ -20320,7 +20311,7 @@
       <c r="I181" s="35"/>
       <c r="J181" s="110"/>
     </row>
-    <row r="182" spans="2:10" ht="18">
+    <row r="182" spans="2:10" ht="17.399999999999999">
       <c r="B182" s="35"/>
       <c r="C182" s="35"/>
       <c r="D182" s="35"/>
@@ -20331,7 +20322,7 @@
       <c r="I182" s="35"/>
       <c r="J182" s="110"/>
     </row>
-    <row r="183" spans="2:10" ht="18">
+    <row r="183" spans="2:10" ht="17.399999999999999">
       <c r="B183" s="35"/>
       <c r="C183" s="35"/>
       <c r="D183" s="35"/>
@@ -20342,7 +20333,7 @@
       <c r="I183" s="35"/>
       <c r="J183" s="110"/>
     </row>
-    <row r="184" spans="2:10" ht="18">
+    <row r="184" spans="2:10" ht="17.399999999999999">
       <c r="B184" s="35"/>
       <c r="C184" s="35"/>
       <c r="D184" s="35"/>
@@ -20353,7 +20344,7 @@
       <c r="I184" s="35"/>
       <c r="J184" s="110"/>
     </row>
-    <row r="185" spans="2:10" ht="18">
+    <row r="185" spans="2:10" ht="17.399999999999999">
       <c r="B185" s="35"/>
       <c r="C185" s="35"/>
       <c r="D185" s="35"/>
@@ -20364,7 +20355,7 @@
       <c r="I185" s="35"/>
       <c r="J185" s="110"/>
     </row>
-    <row r="186" spans="2:10" ht="18">
+    <row r="186" spans="2:10" ht="17.399999999999999">
       <c r="B186" s="35"/>
       <c r="C186" s="35"/>
       <c r="D186" s="34"/>
@@ -20374,7 +20365,7 @@
       <c r="H186" s="34"/>
       <c r="I186" s="37"/>
     </row>
-    <row r="187" spans="2:10" ht="18">
+    <row r="187" spans="2:10" ht="17.399999999999999">
       <c r="B187" s="35"/>
       <c r="C187" s="35"/>
       <c r="D187" s="35"/>
@@ -20385,7 +20376,7 @@
       <c r="I187" s="35"/>
       <c r="J187" s="110"/>
     </row>
-    <row r="188" spans="2:10" ht="18">
+    <row r="188" spans="2:10" ht="17.399999999999999">
       <c r="B188" s="35"/>
       <c r="C188" s="35"/>
       <c r="D188" s="35"/>
@@ -20396,7 +20387,7 @@
       <c r="I188" s="35"/>
       <c r="J188" s="110"/>
     </row>
-    <row r="189" spans="2:10" ht="18">
+    <row r="189" spans="2:10" ht="17.399999999999999">
       <c r="B189" s="35"/>
       <c r="C189" s="35"/>
       <c r="D189" s="35"/>
@@ -20407,7 +20398,7 @@
       <c r="I189" s="35"/>
       <c r="J189" s="110"/>
     </row>
-    <row r="190" spans="2:10" ht="18">
+    <row r="190" spans="2:10" ht="17.399999999999999">
       <c r="B190" s="35"/>
       <c r="C190" s="35"/>
       <c r="D190" s="35"/>
@@ -20418,7 +20409,7 @@
       <c r="I190" s="35"/>
       <c r="J190" s="110"/>
     </row>
-    <row r="191" spans="2:10" ht="18">
+    <row r="191" spans="2:10" ht="17.399999999999999">
       <c r="B191" s="35"/>
       <c r="C191" s="35"/>
       <c r="D191" s="34"/>
@@ -20428,7 +20419,7 @@
       <c r="H191" s="34"/>
       <c r="I191" s="37"/>
     </row>
-    <row r="192" spans="2:10" ht="18">
+    <row r="192" spans="2:10" ht="17.399999999999999">
       <c r="B192" s="37"/>
       <c r="C192" s="37"/>
       <c r="D192" s="37"/>
@@ -20438,7 +20429,7 @@
       <c r="H192" s="37"/>
       <c r="I192" s="37"/>
     </row>
-    <row r="193" spans="2:9" ht="18">
+    <row r="193" spans="2:9" ht="17.399999999999999">
       <c r="B193" s="35"/>
       <c r="C193" s="35"/>
       <c r="D193" s="35"/>
@@ -20448,7 +20439,7 @@
       <c r="H193" s="35"/>
       <c r="I193" s="35"/>
     </row>
-    <row r="194" spans="2:9" ht="18">
+    <row r="194" spans="2:9" ht="17.399999999999999">
       <c r="B194" s="35"/>
       <c r="C194" s="35"/>
       <c r="D194" s="35"/>
@@ -20458,7 +20449,7 @@
       <c r="H194" s="35"/>
       <c r="I194" s="35"/>
     </row>
-    <row r="195" spans="2:9" ht="18">
+    <row r="195" spans="2:9" ht="17.399999999999999">
       <c r="B195" s="35"/>
       <c r="C195" s="35"/>
       <c r="D195" s="34"/>
@@ -20468,7 +20459,7 @@
       <c r="H195" s="34"/>
       <c r="I195" s="37"/>
     </row>
-    <row r="196" spans="2:9" ht="18">
+    <row r="196" spans="2:9" ht="17.399999999999999">
       <c r="B196" s="37"/>
       <c r="C196" s="37"/>
       <c r="D196" s="37"/>
@@ -20478,7 +20469,7 @@
       <c r="H196" s="37"/>
       <c r="I196" s="37"/>
     </row>
-    <row r="197" spans="2:9" ht="18">
+    <row r="197" spans="2:9" ht="17.399999999999999">
       <c r="B197" s="35"/>
       <c r="C197" s="35"/>
       <c r="D197" s="35"/>
@@ -20488,7 +20479,7 @@
       <c r="H197" s="35"/>
       <c r="I197" s="35"/>
     </row>
-    <row r="198" spans="2:9" ht="18">
+    <row r="198" spans="2:9" ht="17.399999999999999">
       <c r="B198" s="35"/>
       <c r="C198" s="35"/>
       <c r="D198" s="35"/>
@@ -20498,7 +20489,7 @@
       <c r="H198" s="35"/>
       <c r="I198" s="35"/>
     </row>
-    <row r="199" spans="2:9" ht="18">
+    <row r="199" spans="2:9" ht="17.399999999999999">
       <c r="B199" s="35"/>
       <c r="C199" s="35"/>
       <c r="D199" s="35"/>
@@ -20508,7 +20499,7 @@
       <c r="H199" s="35"/>
       <c r="I199" s="35"/>
     </row>
-    <row r="200" spans="2:9" ht="18">
+    <row r="200" spans="2:9" ht="17.399999999999999">
       <c r="B200" s="35"/>
       <c r="C200" s="35"/>
       <c r="D200" s="35"/>
@@ -20518,7 +20509,7 @@
       <c r="H200" s="35"/>
       <c r="I200" s="35"/>
     </row>
-    <row r="201" spans="2:9" ht="18">
+    <row r="201" spans="2:9" ht="17.399999999999999">
       <c r="B201" s="35"/>
       <c r="C201" s="35"/>
       <c r="D201" s="35"/>
@@ -20528,7 +20519,7 @@
       <c r="H201" s="35"/>
       <c r="I201" s="35"/>
     </row>
-    <row r="202" spans="2:9" ht="18">
+    <row r="202" spans="2:9" ht="17.399999999999999">
       <c r="B202" s="35"/>
       <c r="C202" s="35"/>
       <c r="D202" s="34"/>
@@ -20538,7 +20529,7 @@
       <c r="H202" s="34"/>
       <c r="I202" s="37"/>
     </row>
-    <row r="203" spans="2:9" ht="18">
+    <row r="203" spans="2:9" ht="17.399999999999999">
       <c r="B203" s="35"/>
       <c r="C203" s="35"/>
       <c r="D203" s="35"/>
@@ -20548,7 +20539,7 @@
       <c r="H203" s="35"/>
       <c r="I203" s="35"/>
     </row>
-    <row r="204" spans="2:9" ht="18">
+    <row r="204" spans="2:9" ht="17.399999999999999">
       <c r="B204" s="35"/>
       <c r="C204" s="35"/>
       <c r="D204" s="35"/>
@@ -20558,7 +20549,7 @@
       <c r="H204" s="35"/>
       <c r="I204" s="35"/>
     </row>
-    <row r="205" spans="2:9" ht="18">
+    <row r="205" spans="2:9" ht="17.399999999999999">
       <c r="B205" s="35"/>
       <c r="C205" s="35"/>
       <c r="D205" s="35"/>
@@ -20568,7 +20559,7 @@
       <c r="H205" s="35"/>
       <c r="I205" s="35"/>
     </row>
-    <row r="206" spans="2:9" ht="18">
+    <row r="206" spans="2:9" ht="17.399999999999999">
       <c r="B206" s="35"/>
       <c r="C206" s="35"/>
       <c r="D206" s="35"/>
@@ -20578,7 +20569,7 @@
       <c r="H206" s="35"/>
       <c r="I206" s="35"/>
     </row>
-    <row r="207" spans="2:9" ht="18">
+    <row r="207" spans="2:9" ht="17.399999999999999">
       <c r="B207" s="35"/>
       <c r="C207" s="35"/>
       <c r="D207" s="35"/>
@@ -20588,7 +20579,7 @@
       <c r="H207" s="35"/>
       <c r="I207" s="35"/>
     </row>
-    <row r="208" spans="2:9" ht="18">
+    <row r="208" spans="2:9" ht="17.399999999999999">
       <c r="B208" s="35"/>
       <c r="C208" s="35"/>
       <c r="D208" s="35"/>
@@ -20598,7 +20589,7 @@
       <c r="H208" s="35"/>
       <c r="I208" s="35"/>
     </row>
-    <row r="209" spans="2:9" ht="18">
+    <row r="209" spans="2:9" ht="17.399999999999999">
       <c r="B209" s="37"/>
       <c r="C209" s="37"/>
       <c r="D209" s="34"/>
@@ -20608,7 +20599,7 @@
       <c r="H209" s="37"/>
       <c r="I209" s="37"/>
     </row>
-    <row r="210" spans="2:9" ht="18">
+    <row r="210" spans="2:9" ht="17.399999999999999">
       <c r="B210" s="40"/>
       <c r="C210" s="40"/>
       <c r="D210" s="40"/>
@@ -20618,7 +20609,7 @@
       <c r="H210" s="40"/>
       <c r="I210" s="40"/>
     </row>
-    <row r="211" spans="2:9" ht="18">
+    <row r="211" spans="2:9" ht="17.399999999999999">
       <c r="B211" s="40"/>
       <c r="C211" s="40"/>
       <c r="D211" s="40"/>
@@ -20628,7 +20619,7 @@
       <c r="H211" s="40"/>
       <c r="I211" s="40"/>
     </row>
-    <row r="212" spans="2:9" ht="18">
+    <row r="212" spans="2:9" ht="17.399999999999999">
       <c r="B212" s="40"/>
       <c r="C212" s="40"/>
       <c r="D212" s="40"/>
@@ -20638,7 +20629,7 @@
       <c r="H212" s="40"/>
       <c r="I212" s="40"/>
     </row>
-    <row r="213" spans="2:9" ht="18">
+    <row r="213" spans="2:9" ht="17.399999999999999">
       <c r="B213" s="35"/>
       <c r="C213" s="35"/>
       <c r="D213" s="35"/>
@@ -20648,7 +20639,7 @@
       <c r="H213" s="35"/>
       <c r="I213" s="35"/>
     </row>
-    <row r="214" spans="2:9" ht="18">
+    <row r="214" spans="2:9" ht="17.399999999999999">
       <c r="B214" s="35"/>
       <c r="C214" s="35"/>
       <c r="D214" s="35"/>
@@ -20658,7 +20649,7 @@
       <c r="H214" s="35"/>
       <c r="I214" s="35"/>
     </row>
-    <row r="215" spans="2:9" ht="18">
+    <row r="215" spans="2:9" ht="17.399999999999999">
       <c r="B215" s="35"/>
       <c r="C215" s="35"/>
       <c r="D215" s="35"/>
@@ -20668,7 +20659,7 @@
       <c r="H215" s="35"/>
       <c r="I215" s="35"/>
     </row>
-    <row r="216" spans="2:9" ht="18">
+    <row r="216" spans="2:9" ht="17.399999999999999">
       <c r="B216" s="35"/>
       <c r="C216" s="35"/>
       <c r="D216" s="35"/>
@@ -20678,7 +20669,7 @@
       <c r="H216" s="35"/>
       <c r="I216" s="35"/>
     </row>
-    <row r="217" spans="2:9" ht="18">
+    <row r="217" spans="2:9" ht="17.399999999999999">
       <c r="B217" s="35"/>
       <c r="C217" s="35"/>
       <c r="D217" s="35"/>
@@ -20688,7 +20679,7 @@
       <c r="H217" s="35"/>
       <c r="I217" s="35"/>
     </row>
-    <row r="218" spans="2:9" ht="18">
+    <row r="218" spans="2:9" ht="17.399999999999999">
       <c r="B218" s="35"/>
       <c r="C218" s="35"/>
       <c r="D218" s="35"/>
@@ -20698,7 +20689,7 @@
       <c r="H218" s="35"/>
       <c r="I218" s="35"/>
     </row>
-    <row r="219" spans="2:9" ht="18">
+    <row r="219" spans="2:9" ht="17.399999999999999">
       <c r="B219" s="35"/>
       <c r="C219" s="35"/>
       <c r="D219" s="35"/>
@@ -20708,7 +20699,7 @@
       <c r="H219" s="35"/>
       <c r="I219" s="35"/>
     </row>
-    <row r="220" spans="2:9" ht="18">
+    <row r="220" spans="2:9" ht="17.399999999999999">
       <c r="B220" s="35"/>
       <c r="C220" s="35"/>
       <c r="D220" s="34"/>
@@ -20718,7 +20709,7 @@
       <c r="H220" s="34"/>
       <c r="I220" s="37"/>
     </row>
-    <row r="221" spans="2:9" ht="18">
+    <row r="221" spans="2:9" ht="17.399999999999999">
       <c r="B221" s="37"/>
       <c r="C221" s="37"/>
       <c r="D221" s="37"/>
@@ -20728,7 +20719,7 @@
       <c r="H221" s="37"/>
       <c r="I221" s="37"/>
     </row>
-    <row r="222" spans="2:9" ht="18">
+    <row r="222" spans="2:9" ht="17.399999999999999">
       <c r="B222" s="35"/>
       <c r="C222" s="35"/>
       <c r="D222" s="35"/>
@@ -20738,7 +20729,7 @@
       <c r="H222" s="35"/>
       <c r="I222" s="35"/>
     </row>
-    <row r="223" spans="2:9" ht="18">
+    <row r="223" spans="2:9" ht="17.399999999999999">
       <c r="B223" s="35"/>
       <c r="C223" s="35"/>
       <c r="D223" s="35"/>
@@ -20748,7 +20739,7 @@
       <c r="H223" s="35"/>
       <c r="I223" s="35"/>
     </row>
-    <row r="224" spans="2:9" ht="18">
+    <row r="224" spans="2:9" ht="17.399999999999999">
       <c r="B224" s="35"/>
       <c r="C224" s="35"/>
       <c r="D224" s="35"/>
@@ -20758,7 +20749,7 @@
       <c r="H224" s="35"/>
       <c r="I224" s="35"/>
     </row>
-    <row r="225" spans="2:9" ht="18">
+    <row r="225" spans="2:9" ht="17.399999999999999">
       <c r="B225" s="35"/>
       <c r="C225" s="35"/>
       <c r="D225" s="35"/>
@@ -20768,7 +20759,7 @@
       <c r="H225" s="35"/>
       <c r="I225" s="35"/>
     </row>
-    <row r="226" spans="2:9" ht="18">
+    <row r="226" spans="2:9" ht="17.399999999999999">
       <c r="B226" s="35"/>
       <c r="C226" s="35"/>
       <c r="D226" s="35"/>
@@ -20778,7 +20769,7 @@
       <c r="H226" s="35"/>
       <c r="I226" s="35"/>
     </row>
-    <row r="227" spans="2:9" ht="18">
+    <row r="227" spans="2:9" ht="17.399999999999999">
       <c r="B227" s="35"/>
       <c r="C227" s="35"/>
       <c r="D227" s="35"/>
@@ -20788,7 +20779,7 @@
       <c r="H227" s="35"/>
       <c r="I227" s="35"/>
     </row>
-    <row r="228" spans="2:9" ht="18">
+    <row r="228" spans="2:9" ht="17.399999999999999">
       <c r="B228" s="35"/>
       <c r="C228" s="35"/>
       <c r="D228" s="35"/>
@@ -20798,7 +20789,7 @@
       <c r="H228" s="35"/>
       <c r="I228" s="35"/>
     </row>
-    <row r="229" spans="2:9" ht="18">
+    <row r="229" spans="2:9" ht="17.399999999999999">
       <c r="B229" s="35"/>
       <c r="C229" s="35"/>
       <c r="D229" s="35"/>
@@ -20808,7 +20799,7 @@
       <c r="H229" s="35"/>
       <c r="I229" s="35"/>
     </row>
-    <row r="230" spans="2:9" ht="18">
+    <row r="230" spans="2:9" ht="17.399999999999999">
       <c r="B230" s="35"/>
       <c r="C230" s="35"/>
       <c r="D230" s="35"/>
@@ -20818,7 +20809,7 @@
       <c r="H230" s="35"/>
       <c r="I230" s="35"/>
     </row>
-    <row r="231" spans="2:9" ht="18">
+    <row r="231" spans="2:9" ht="17.399999999999999">
       <c r="B231" s="35"/>
       <c r="C231" s="35"/>
       <c r="D231" s="35"/>
@@ -20828,7 +20819,7 @@
       <c r="H231" s="35"/>
       <c r="I231" s="82"/>
     </row>
-    <row r="232" spans="2:9" ht="18">
+    <row r="232" spans="2:9" ht="17.399999999999999">
       <c r="B232" s="35"/>
       <c r="C232" s="35"/>
       <c r="D232" s="35"/>
@@ -20838,7 +20829,7 @@
       <c r="H232" s="35"/>
       <c r="I232" s="82"/>
     </row>
-    <row r="233" spans="2:9" ht="18">
+    <row r="233" spans="2:9" ht="17.399999999999999">
       <c r="B233" s="35"/>
       <c r="C233" s="35"/>
       <c r="D233" s="35"/>
@@ -20848,7 +20839,7 @@
       <c r="H233" s="35"/>
       <c r="I233" s="82"/>
     </row>
-    <row r="234" spans="2:9" ht="18">
+    <row r="234" spans="2:9" ht="17.399999999999999">
       <c r="B234" s="35"/>
       <c r="C234" s="35"/>
       <c r="D234" s="35"/>
@@ -20858,7 +20849,7 @@
       <c r="H234" s="35"/>
       <c r="I234" s="35"/>
     </row>
-    <row r="236" spans="2:9" ht="18">
+    <row r="236" spans="2:9" ht="17.399999999999999">
       <c r="B236" s="35"/>
       <c r="C236" s="35"/>
       <c r="D236" s="35"/>
@@ -20868,7 +20859,7 @@
       <c r="H236" s="35"/>
       <c r="I236" s="35"/>
     </row>
-    <row r="237" spans="2:9" ht="18">
+    <row r="237" spans="2:9" ht="17.399999999999999">
       <c r="B237" s="35"/>
       <c r="C237" s="35"/>
       <c r="D237" s="35"/>
@@ -20878,7 +20869,7 @@
       <c r="H237" s="35"/>
       <c r="I237" s="35"/>
     </row>
-    <row r="238" spans="2:9" ht="18">
+    <row r="238" spans="2:9" ht="17.399999999999999">
       <c r="B238" s="35"/>
       <c r="C238" s="35"/>
       <c r="D238" s="35"/>
@@ -27162,28 +27153,28 @@
       <selection activeCell="L175" sqref="L175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="35" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="35" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="35" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="35" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="35" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="103" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="35" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="35" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="37" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="35" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" style="35" customWidth="1"/>
-    <col min="15" max="15" width="3.7109375" style="35" customWidth="1"/>
-    <col min="16" max="16" width="2.7109375" style="35" customWidth="1"/>
-    <col min="17" max="16384" width="8.85546875" style="35"/>
+    <col min="4" max="4" width="5.6640625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" style="35" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" style="35" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" style="35" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="103" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" style="35" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" style="35" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" style="37" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" style="35" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" style="35" customWidth="1"/>
+    <col min="15" max="15" width="3.6640625" style="35" customWidth="1"/>
+    <col min="16" max="16" width="2.6640625" style="35" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="32.25">
+    <row r="1" spans="2:24" ht="31.8">
       <c r="E1" s="31" t="s">
         <v>0</v>
       </c>
@@ -27198,7 +27189,7 @@
       <c r="I2" s="113"/>
       <c r="J2" s="37"/>
     </row>
-    <row r="3" spans="2:24" ht="32.25">
+    <row r="3" spans="2:24" ht="31.8">
       <c r="E3" s="69" t="s">
         <v>1</v>
       </c>
@@ -27207,7 +27198,7 @@
       <c r="I3" s="114"/>
       <c r="J3" s="37"/>
     </row>
-    <row r="4" spans="2:24" ht="10.15" customHeight="1">
+    <row r="4" spans="2:24" ht="10.199999999999999" customHeight="1">
       <c r="E4" s="68"/>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
@@ -27215,7 +27206,7 @@
       <c r="I4" s="114"/>
       <c r="J4" s="37"/>
     </row>
-    <row r="5" spans="2:24" ht="32.25">
+    <row r="5" spans="2:24" ht="31.8">
       <c r="E5" s="70" t="s">
         <v>561</v>
       </c>
@@ -27235,7 +27226,7 @@
       <c r="G6" s="34"/>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="2:24" ht="19.899999999999999" customHeight="1">
+    <row r="7" spans="2:24" ht="19.95" customHeight="1">
       <c r="B7" s="25" t="s">
         <v>3</v>
       </c>
@@ -27275,7 +27266,7 @@
       <c r="W7" s="83"/>
       <c r="X7" s="83"/>
     </row>
-    <row r="8" spans="2:24" ht="19.899999999999999" customHeight="1">
+    <row r="8" spans="2:24" ht="19.95" customHeight="1">
       <c r="B8" s="25"/>
       <c r="C8" s="22" t="s">
         <v>651</v>
@@ -27293,7 +27284,7 @@
       <c r="N8" s="22"/>
       <c r="O8" s="20"/>
     </row>
-    <row r="9" spans="2:24" ht="18.75">
+    <row r="9" spans="2:24">
       <c r="B9" s="20"/>
       <c r="C9" s="78" t="s">
         <v>777</v>
@@ -27311,7 +27302,7 @@
       <c r="N9" s="22"/>
       <c r="O9" s="20"/>
     </row>
-    <row r="10" spans="2:24" ht="18.75" hidden="1">
+    <row r="10" spans="2:24" hidden="1">
       <c r="B10" s="35" t="s">
         <v>8</v>
       </c>
@@ -27337,7 +27328,7 @@
       </c>
       <c r="O10" s="34"/>
     </row>
-    <row r="11" spans="2:24" ht="18.75" hidden="1">
+    <row r="11" spans="2:24" hidden="1">
       <c r="B11" s="35" t="s">
         <v>11</v>
       </c>
@@ -27357,7 +27348,7 @@
       <c r="N11" s="44"/>
       <c r="O11" s="34"/>
     </row>
-    <row r="12" spans="2:24" ht="18.75" hidden="1">
+    <row r="12" spans="2:24" hidden="1">
       <c r="B12" s="35" t="s">
         <v>13</v>
       </c>
@@ -27383,7 +27374,7 @@
       </c>
       <c r="O12" s="34"/>
     </row>
-    <row r="13" spans="2:24" ht="18.75" hidden="1">
+    <row r="13" spans="2:24" hidden="1">
       <c r="B13" s="35" t="s">
         <v>16</v>
       </c>
@@ -27409,7 +27400,7 @@
       </c>
       <c r="O13" s="34"/>
     </row>
-    <row r="14" spans="2:24" ht="18.75" hidden="1">
+    <row r="14" spans="2:24" hidden="1">
       <c r="B14" s="35" t="s">
         <v>398</v>
       </c>
@@ -27435,7 +27426,7 @@
       </c>
       <c r="O14" s="34"/>
     </row>
-    <row r="15" spans="2:24" ht="18.75" hidden="1">
+    <row r="15" spans="2:24" hidden="1">
       <c r="B15" s="35" t="s">
         <v>485</v>
       </c>
@@ -27455,7 +27446,7 @@
       <c r="N15" s="44"/>
       <c r="O15" s="34"/>
     </row>
-    <row r="16" spans="2:24" ht="18.75" hidden="1">
+    <row r="16" spans="2:24" hidden="1">
       <c r="B16" s="35" t="s">
         <v>503</v>
       </c>
@@ -27475,7 +27466,7 @@
       <c r="N16" s="44"/>
       <c r="O16" s="34"/>
     </row>
-    <row r="17" spans="2:15" ht="18.75" hidden="1">
+    <row r="17" spans="2:15" hidden="1">
       <c r="B17" s="35" t="s">
         <v>504</v>
       </c>
@@ -27495,7 +27486,7 @@
       <c r="N17" s="44"/>
       <c r="O17" s="34"/>
     </row>
-    <row r="18" spans="2:15" ht="18.75" hidden="1">
+    <row r="18" spans="2:15" hidden="1">
       <c r="B18" s="37" t="s">
         <v>650</v>
       </c>
@@ -27521,7 +27512,7 @@
       </c>
       <c r="O18" s="34"/>
     </row>
-    <row r="19" spans="2:15" ht="18.75">
+    <row r="19" spans="2:15">
       <c r="B19" s="37"/>
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
@@ -27633,7 +27624,7 @@
       <c r="N22" s="44"/>
       <c r="O22" s="34"/>
     </row>
-    <row r="23" spans="2:15" ht="16.899999999999999" customHeight="1">
+    <row r="23" spans="2:15" ht="16.95" customHeight="1">
       <c r="B23" s="35" t="s">
         <v>26</v>
       </c>
@@ -27665,7 +27656,7 @@
       <c r="N23" s="44"/>
       <c r="O23" s="34"/>
     </row>
-    <row r="24" spans="2:15" ht="16.899999999999999" customHeight="1">
+    <row r="24" spans="2:15" ht="16.95" customHeight="1">
       <c r="B24" s="35" t="s">
         <v>16</v>
       </c>
@@ -27697,7 +27688,7 @@
       <c r="N24" s="44"/>
       <c r="O24" s="34"/>
     </row>
-    <row r="25" spans="2:15" ht="16.899999999999999" customHeight="1">
+    <row r="25" spans="2:15" ht="16.95" customHeight="1">
       <c r="B25" s="35" t="s">
         <v>485</v>
       </c>
@@ -27729,7 +27720,7 @@
       <c r="N25" s="44"/>
       <c r="O25" s="34"/>
     </row>
-    <row r="26" spans="2:15" ht="16.899999999999999" customHeight="1">
+    <row r="26" spans="2:15" ht="16.95" customHeight="1">
       <c r="B26" s="35" t="s">
         <v>503</v>
       </c>
@@ -27761,7 +27752,7 @@
       <c r="N26" s="44"/>
       <c r="O26" s="34"/>
     </row>
-    <row r="27" spans="2:15" ht="16.899999999999999" customHeight="1">
+    <row r="27" spans="2:15" ht="16.95" customHeight="1">
       <c r="B27" s="35" t="s">
         <v>722</v>
       </c>
@@ -27780,7 +27771,7 @@
         <v>579</v>
       </c>
       <c r="I27" s="114" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="J27" s="44" t="s">
         <v>834</v>
@@ -28147,7 +28138,7 @@
       <c r="N38" s="44"/>
       <c r="O38" s="34"/>
     </row>
-    <row r="39" spans="2:15" ht="18.75">
+    <row r="39" spans="2:15">
       <c r="C39" s="34"/>
       <c r="D39" s="34"/>
       <c r="E39" s="44"/>
@@ -28433,7 +28424,7 @@
         <v>25</v>
       </c>
       <c r="I49" s="114" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="J49" s="44" t="s">
         <v>834</v>
@@ -28442,7 +28433,7 @@
         <v>882</v>
       </c>
       <c r="L49" s="40" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="50" spans="2:12">
@@ -28734,7 +28725,7 @@
       </c>
       <c r="D60" s="34"/>
       <c r="E60" s="40" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F60" s="34">
         <v>1987</v>
@@ -28753,7 +28744,7 @@
         <v>882</v>
       </c>
       <c r="L60" s="37" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="61" spans="2:12">
@@ -29089,7 +29080,7 @@
         <v>25</v>
       </c>
       <c r="I73" s="114" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="J73" s="44" t="s">
         <v>834</v>
@@ -29118,7 +29109,7 @@
         <v>25</v>
       </c>
       <c r="I74" s="114" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="J74" s="44" t="s">
         <v>834</v>
@@ -29127,7 +29118,7 @@
         <v>883</v>
       </c>
       <c r="L74" s="40" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="75" spans="2:18">
@@ -29691,7 +29682,7 @@
         <v>25</v>
       </c>
       <c r="I95" s="114" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="J95" s="44" t="s">
         <v>834</v>
@@ -30731,7 +30722,7 @@
         <v>885</v>
       </c>
       <c r="L132" s="37" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="133" spans="2:12">
@@ -30846,7 +30837,7 @@
         <v>885</v>
       </c>
       <c r="L136" s="37" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="137" spans="2:12">
@@ -30877,7 +30868,7 @@
         <v>885</v>
       </c>
       <c r="L137" s="37" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="138" spans="2:12">
@@ -31583,7 +31574,7 @@
         <v>886</v>
       </c>
       <c r="L163" s="37" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="164" spans="2:12">
@@ -31614,7 +31605,7 @@
         <v>886</v>
       </c>
       <c r="L164" s="37" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="165" spans="2:12">
@@ -31768,7 +31759,7 @@
         <v>887</v>
       </c>
       <c r="L170" s="37" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="171" spans="2:12">
@@ -31799,7 +31790,7 @@
         <v>887</v>
       </c>
       <c r="L171" s="37" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="172" spans="2:12">
@@ -31830,7 +31821,7 @@
         <v>887</v>
       </c>
       <c r="L172" s="37" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="173" spans="2:12">
@@ -31861,7 +31852,7 @@
         <v>887</v>
       </c>
       <c r="L173" s="37" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="174" spans="2:12">
@@ -31892,7 +31883,7 @@
         <v>887</v>
       </c>
       <c r="L174" s="37" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="175" spans="2:12">
@@ -37582,20 +37573,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:K1456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K150" sqref="K150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" customWidth="1"/>
     <col min="5" max="5" width="19" style="7" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="108"/>
+    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" style="108"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="30" customHeight="1">
@@ -37608,15 +37599,15 @@
       <c r="E2" s="11"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="2:10" ht="25.5">
+    <row r="3" spans="2:10" ht="24.6">
       <c r="E3" s="29" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="10.9" customHeight="1">
+    <row r="4" spans="2:10" ht="10.95" customHeight="1">
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="2:10" ht="25.5">
+    <row r="5" spans="2:10" ht="24.6">
       <c r="E5" s="24" t="s">
         <v>389</v>
       </c>
@@ -37624,10 +37615,10 @@
         <v>764</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="10.15" customHeight="1">
+    <row r="6" spans="2:10" ht="10.199999999999999" customHeight="1">
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="2:10" s="28" customFormat="1" ht="20.25">
+    <row r="7" spans="2:10" s="28" customFormat="1" ht="20.399999999999999">
       <c r="B7" s="25" t="s">
         <v>3</v>
       </c>
@@ -37654,7 +37645,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="10.15" customHeight="1">
+    <row r="8" spans="2:10" ht="10.199999999999999" customHeight="1">
       <c r="B8" s="13"/>
       <c r="C8" s="15"/>
       <c r="D8" s="13"/>
@@ -37662,7 +37653,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="2:10" ht="18">
+    <row r="9" spans="2:10" ht="17.399999999999999">
       <c r="B9" s="35" t="s">
         <v>8</v>
       </c>
@@ -37689,7 +37680,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="18">
+    <row r="10" spans="2:10" ht="17.399999999999999">
       <c r="B10" s="35" t="s">
         <v>11</v>
       </c>
@@ -37716,7 +37707,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="18">
+    <row r="11" spans="2:10" ht="17.399999999999999">
       <c r="B11" s="35" t="s">
         <v>13</v>
       </c>
@@ -37743,7 +37734,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="18">
+    <row r="12" spans="2:10" ht="17.399999999999999">
       <c r="B12" s="35" t="s">
         <v>16</v>
       </c>
@@ -37770,7 +37761,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="18">
+    <row r="13" spans="2:10" ht="17.399999999999999">
       <c r="B13" s="35" t="s">
         <v>398</v>
       </c>
@@ -37797,7 +37788,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="18">
+    <row r="14" spans="2:10" ht="17.399999999999999">
       <c r="B14" s="35" t="s">
         <v>485</v>
       </c>
@@ -37824,7 +37815,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="18">
+    <row r="15" spans="2:10" ht="17.399999999999999">
       <c r="B15" s="35" t="s">
         <v>503</v>
       </c>
@@ -37851,7 +37842,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="18">
+    <row r="16" spans="2:10" ht="17.399999999999999">
       <c r="B16" s="35" t="s">
         <v>65</v>
       </c>
@@ -37878,7 +37869,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="18">
+    <row r="17" spans="2:10" ht="17.399999999999999">
       <c r="B17" s="40" t="s">
         <v>26</v>
       </c>
@@ -37905,7 +37896,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="18">
+    <row r="18" spans="2:10" ht="17.399999999999999">
       <c r="B18" s="35" t="s">
         <v>34</v>
       </c>
@@ -37932,7 +37923,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="18">
+    <row r="19" spans="2:10" ht="17.399999999999999">
       <c r="B19" s="35" t="s">
         <v>36</v>
       </c>
@@ -37959,7 +37950,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="18">
+    <row r="20" spans="2:10" ht="17.399999999999999">
       <c r="B20" s="35" t="s">
         <v>31</v>
       </c>
@@ -37986,7 +37977,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="18">
+    <row r="21" spans="2:10" ht="17.399999999999999">
       <c r="B21" s="35" t="s">
         <v>39</v>
       </c>
@@ -38013,7 +38004,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="18">
+    <row r="22" spans="2:10" ht="17.399999999999999">
       <c r="B22" s="35" t="s">
         <v>42</v>
       </c>
@@ -38040,7 +38031,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="18">
+    <row r="23" spans="2:10" ht="17.399999999999999">
       <c r="B23" s="35" t="s">
         <v>44</v>
       </c>
@@ -38067,7 +38058,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="18">
+    <row r="24" spans="2:10" ht="17.399999999999999">
       <c r="B24" s="35" t="s">
         <v>219</v>
       </c>
@@ -38094,7 +38085,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="18">
+    <row r="25" spans="2:10" ht="17.399999999999999">
       <c r="B25" s="35" t="s">
         <v>222</v>
       </c>
@@ -38121,7 +38112,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="18">
+    <row r="26" spans="2:10" ht="17.399999999999999">
       <c r="B26" s="35" t="s">
         <v>49</v>
       </c>
@@ -38148,7 +38139,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="18">
+    <row r="27" spans="2:10" ht="17.399999999999999">
       <c r="B27" s="35" t="s">
         <v>528</v>
       </c>
@@ -38175,7 +38166,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="18">
+    <row r="28" spans="2:10" ht="17.399999999999999">
       <c r="B28" s="35" t="s">
         <v>733</v>
       </c>
@@ -38202,7 +38193,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="18">
+    <row r="29" spans="2:10" ht="17.399999999999999">
       <c r="B29" s="35"/>
       <c r="C29" s="34"/>
       <c r="D29" s="35"/>
@@ -38210,7 +38201,7 @@
       <c r="F29" s="34"/>
       <c r="G29" s="40"/>
     </row>
-    <row r="30" spans="2:10" ht="18">
+    <row r="30" spans="2:10" ht="17.399999999999999">
       <c r="B30" s="35" t="s">
         <v>8</v>
       </c>
@@ -38237,7 +38228,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="18">
+    <row r="31" spans="2:10" ht="17.399999999999999">
       <c r="B31" s="35" t="s">
         <v>11</v>
       </c>
@@ -38264,7 +38255,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="18">
+    <row r="32" spans="2:10" ht="17.399999999999999">
       <c r="B32" s="41" t="s">
         <v>13</v>
       </c>
@@ -38291,7 +38282,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="18">
+    <row r="33" spans="2:10" ht="17.399999999999999">
       <c r="B33" s="41" t="s">
         <v>16</v>
       </c>
@@ -38318,7 +38309,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="18">
+    <row r="34" spans="2:10" ht="17.399999999999999">
       <c r="B34" s="41" t="s">
         <v>398</v>
       </c>
@@ -38345,7 +38336,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="18">
+    <row r="35" spans="2:10" ht="17.399999999999999">
       <c r="B35" s="41" t="s">
         <v>485</v>
       </c>
@@ -38360,7 +38351,7 @@
         <v>2002</v>
       </c>
       <c r="G35" s="44" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H35" s="112" t="s">
         <v>844</v>
@@ -38372,7 +38363,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="18">
+    <row r="36" spans="2:10" ht="17.399999999999999">
       <c r="B36" s="41" t="s">
         <v>503</v>
       </c>
@@ -38399,7 +38390,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="37" spans="2:10" ht="18">
+    <row r="37" spans="2:10" ht="17.399999999999999">
       <c r="B37" s="41" t="s">
         <v>65</v>
       </c>
@@ -38426,7 +38417,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="18">
+    <row r="38" spans="2:10" ht="17.399999999999999">
       <c r="B38" s="41" t="s">
         <v>404</v>
       </c>
@@ -38453,7 +38444,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="18">
+    <row r="39" spans="2:10" ht="17.399999999999999">
       <c r="B39" s="41" t="s">
         <v>26</v>
       </c>
@@ -38480,7 +38471,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="40" spans="2:10" ht="18">
+    <row r="40" spans="2:10" ht="17.399999999999999">
       <c r="B40" s="41" t="s">
         <v>34</v>
       </c>
@@ -38507,7 +38498,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="41" spans="2:10" ht="18">
+    <row r="41" spans="2:10" ht="17.399999999999999">
       <c r="B41" s="41" t="s">
         <v>36</v>
       </c>
@@ -38534,7 +38525,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="18">
+    <row r="42" spans="2:10" ht="17.399999999999999">
       <c r="B42" s="41" t="s">
         <v>31</v>
       </c>
@@ -38561,7 +38552,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="43" spans="2:10" ht="18">
+    <row r="43" spans="2:10" ht="17.399999999999999">
       <c r="B43" s="41" t="s">
         <v>39</v>
       </c>
@@ -38588,7 +38579,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="44" spans="2:10" ht="18">
+    <row r="44" spans="2:10" ht="17.399999999999999">
       <c r="B44" s="41" t="s">
         <v>42</v>
       </c>
@@ -38615,7 +38606,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="18">
+    <row r="45" spans="2:10" ht="17.399999999999999">
       <c r="B45" s="41" t="s">
         <v>44</v>
       </c>
@@ -38642,7 +38633,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="46" spans="2:10" ht="18">
+    <row r="46" spans="2:10" ht="17.399999999999999">
       <c r="B46" s="41" t="s">
         <v>219</v>
       </c>
@@ -38669,7 +38660,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="47" spans="2:10" ht="18">
+    <row r="47" spans="2:10" ht="17.399999999999999">
       <c r="B47" s="41" t="s">
         <v>222</v>
       </c>
@@ -38696,7 +38687,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="48" spans="2:10" ht="18">
+    <row r="48" spans="2:10" ht="17.399999999999999">
       <c r="B48" s="41" t="s">
         <v>49</v>
       </c>
@@ -38723,7 +38714,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="49" spans="2:11" ht="13.9" customHeight="1">
+    <row r="49" spans="2:11" ht="13.95" customHeight="1">
       <c r="B49" s="20"/>
       <c r="C49" s="76"/>
       <c r="D49" s="20"/>
@@ -38732,7 +38723,7 @@
       <c r="G49" s="22"/>
       <c r="I49" s="9"/>
     </row>
-    <row r="50" spans="2:11" ht="18">
+    <row r="50" spans="2:11" ht="17.399999999999999">
       <c r="B50" s="41" t="s">
         <v>8</v>
       </c>
@@ -38759,7 +38750,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="18">
+    <row r="51" spans="2:11" ht="17.399999999999999">
       <c r="B51" s="43" t="s">
         <v>11</v>
       </c>
@@ -38786,7 +38777,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="18">
+    <row r="52" spans="2:11" ht="17.399999999999999">
       <c r="B52" s="41" t="s">
         <v>13</v>
       </c>
@@ -38801,7 +38792,7 @@
         <v>2006</v>
       </c>
       <c r="G52" s="44" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H52" s="112" t="s">
         <v>841</v>
@@ -38813,7 +38804,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="18">
+    <row r="53" spans="2:11" ht="17.399999999999999">
       <c r="B53" s="41" t="s">
         <v>16</v>
       </c>
@@ -38822,13 +38813,13 @@
       </c>
       <c r="D53" s="41"/>
       <c r="E53" s="106" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F53" s="42">
         <v>2006</v>
       </c>
       <c r="G53" s="44" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H53" s="112" t="s">
         <v>842</v>
@@ -38840,10 +38831,10 @@
         <v>883</v>
       </c>
       <c r="K53" s="84" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" ht="18">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" ht="17.399999999999999">
       <c r="B54" s="41" t="s">
         <v>398</v>
       </c>
@@ -38858,7 +38849,7 @@
         <v>2006</v>
       </c>
       <c r="G54" s="44" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H54" s="112" t="s">
         <v>843</v>
@@ -38870,10 +38861,10 @@
         <v>883</v>
       </c>
       <c r="K54" s="84" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11" ht="18">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" ht="17.399999999999999">
       <c r="B55" s="41" t="s">
         <v>485</v>
       </c>
@@ -38888,7 +38879,7 @@
         <v>2006</v>
       </c>
       <c r="G55" s="44" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H55" s="112" t="s">
         <v>844</v>
@@ -38900,7 +38891,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="56" spans="2:11" s="33" customFormat="1" ht="18">
+    <row r="56" spans="2:11" s="33" customFormat="1" ht="17.399999999999999">
       <c r="B56" s="41" t="s">
         <v>503</v>
       </c>
@@ -38927,7 +38918,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="57" spans="2:11" ht="18">
+    <row r="57" spans="2:11" ht="17.399999999999999">
       <c r="B57" s="41" t="s">
         <v>504</v>
       </c>
@@ -38954,7 +38945,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="58" spans="2:11" ht="18">
+    <row r="58" spans="2:11" ht="17.399999999999999">
       <c r="B58" s="41" t="s">
         <v>65</v>
       </c>
@@ -38981,7 +38972,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="18">
+    <row r="59" spans="2:11" ht="17.399999999999999">
       <c r="B59" s="41" t="s">
         <v>456</v>
       </c>
@@ -39008,7 +38999,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="18">
+    <row r="60" spans="2:11" ht="17.399999999999999">
       <c r="B60" s="41" t="s">
         <v>26</v>
       </c>
@@ -39035,7 +39026,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="18">
+    <row r="61" spans="2:11" ht="17.399999999999999">
       <c r="B61" s="41" t="s">
         <v>34</v>
       </c>
@@ -39062,7 +39053,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="62" spans="2:11" ht="18">
+    <row r="62" spans="2:11" ht="17.399999999999999">
       <c r="B62" s="41" t="s">
         <v>31</v>
       </c>
@@ -39089,7 +39080,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="63" spans="2:11" ht="18">
+    <row r="63" spans="2:11" ht="17.399999999999999">
       <c r="B63" s="41" t="s">
         <v>42</v>
       </c>
@@ -39116,7 +39107,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="64" spans="2:11" ht="18">
+    <row r="64" spans="2:11" ht="17.399999999999999">
       <c r="B64" s="41" t="s">
         <v>44</v>
       </c>
@@ -39143,7 +39134,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="18">
+    <row r="65" spans="2:11" ht="17.399999999999999">
       <c r="B65" s="43" t="s">
         <v>222</v>
       </c>
@@ -39170,7 +39161,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="66" spans="2:11" ht="18">
+    <row r="66" spans="2:11" ht="17.399999999999999">
       <c r="B66" s="41" t="s">
         <v>49</v>
       </c>
@@ -39197,7 +39188,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="67" spans="2:11" ht="17.45" customHeight="1">
+    <row r="67" spans="2:11" ht="17.399999999999999" customHeight="1">
       <c r="B67" s="43"/>
       <c r="C67" s="34"/>
       <c r="D67" s="41"/>
@@ -39206,7 +39197,7 @@
       <c r="G67" s="43"/>
       <c r="I67" s="9"/>
     </row>
-    <row r="68" spans="2:11" ht="17.45" customHeight="1">
+    <row r="68" spans="2:11" ht="17.399999999999999" customHeight="1">
       <c r="B68" s="41" t="s">
         <v>8</v>
       </c>
@@ -39233,7 +39224,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="69" spans="2:11" ht="17.45" customHeight="1">
+    <row r="69" spans="2:11" ht="17.399999999999999" customHeight="1">
       <c r="B69" s="41" t="s">
         <v>11</v>
       </c>
@@ -39260,7 +39251,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="70" spans="2:11" ht="18">
+    <row r="70" spans="2:11" ht="17.399999999999999">
       <c r="B70" s="41" t="s">
         <v>13</v>
       </c>
@@ -39287,7 +39278,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="71" spans="2:11" ht="18">
+    <row r="71" spans="2:11" ht="17.399999999999999">
       <c r="B71" s="41" t="s">
         <v>16</v>
       </c>
@@ -39314,7 +39305,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="72" spans="2:11" ht="18">
+    <row r="72" spans="2:11" ht="17.399999999999999">
       <c r="B72" s="41" t="s">
         <v>398</v>
       </c>
@@ -39341,7 +39332,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="73" spans="2:11" ht="18">
+    <row r="73" spans="2:11" ht="17.399999999999999">
       <c r="B73" s="41" t="s">
         <v>485</v>
       </c>
@@ -39368,7 +39359,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="74" spans="2:11" ht="18">
+    <row r="74" spans="2:11" ht="17.399999999999999">
       <c r="B74" s="41" t="s">
         <v>503</v>
       </c>
@@ -39395,7 +39386,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="75" spans="2:11" ht="18">
+    <row r="75" spans="2:11" ht="17.399999999999999">
       <c r="B75" s="41" t="s">
         <v>34</v>
       </c>
@@ -39422,7 +39413,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="76" spans="2:11" ht="18">
+    <row r="76" spans="2:11" ht="17.399999999999999">
       <c r="B76" s="41" t="s">
         <v>407</v>
       </c>
@@ -39449,7 +39440,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="77" spans="2:11" ht="18">
+    <row r="77" spans="2:11" ht="17.399999999999999">
       <c r="B77" s="41" t="s">
         <v>408</v>
       </c>
@@ -39476,7 +39467,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="78" spans="2:11" ht="18">
+    <row r="78" spans="2:11" ht="17.399999999999999">
       <c r="B78" s="41" t="s">
         <v>44</v>
       </c>
@@ -39503,7 +39494,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="79" spans="2:11" ht="18">
+    <row r="79" spans="2:11" ht="17.399999999999999">
       <c r="B79" s="41" t="s">
         <v>219</v>
       </c>
@@ -39530,10 +39521,10 @@
         <v>884</v>
       </c>
       <c r="K79" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="80" spans="2:11" ht="18">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" ht="17.399999999999999">
       <c r="B80" s="41" t="s">
         <v>222</v>
       </c>
@@ -39560,10 +39551,10 @@
         <v>884</v>
       </c>
       <c r="K80" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10" ht="18">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" ht="17.399999999999999">
       <c r="B81" s="41" t="s">
         <v>414</v>
       </c>
@@ -39590,7 +39581,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="82" spans="2:10" ht="18">
+    <row r="82" spans="2:10" ht="17.399999999999999">
       <c r="B82" s="41" t="s">
         <v>416</v>
       </c>
@@ -39617,7 +39608,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="83" spans="2:10" ht="18">
+    <row r="83" spans="2:10" ht="17.399999999999999">
       <c r="B83" s="41" t="s">
         <v>528</v>
       </c>
@@ -39644,7 +39635,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="84" spans="2:10" ht="18">
+    <row r="84" spans="2:10" ht="17.399999999999999">
       <c r="B84" s="41"/>
       <c r="C84" s="42"/>
       <c r="D84" s="41"/>
@@ -39652,7 +39643,7 @@
       <c r="F84" s="42"/>
       <c r="G84" s="44"/>
     </row>
-    <row r="85" spans="2:10" ht="18">
+    <row r="85" spans="2:10" ht="17.399999999999999">
       <c r="B85" s="41" t="s">
         <v>8</v>
       </c>
@@ -39679,7 +39670,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="86" spans="2:10" ht="18">
+    <row r="86" spans="2:10" ht="17.399999999999999">
       <c r="B86" s="41" t="s">
         <v>11</v>
       </c>
@@ -39706,7 +39697,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="87" spans="2:10" ht="18">
+    <row r="87" spans="2:10" ht="17.399999999999999">
       <c r="B87" s="41" t="s">
         <v>13</v>
       </c>
@@ -39733,7 +39724,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="88" spans="2:10" ht="18">
+    <row r="88" spans="2:10" ht="17.399999999999999">
       <c r="B88" s="43" t="s">
         <v>16</v>
       </c>
@@ -39760,7 +39751,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="89" spans="2:10" ht="18">
+    <row r="89" spans="2:10" ht="17.399999999999999">
       <c r="B89" s="43" t="s">
         <v>398</v>
       </c>
@@ -39787,7 +39778,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="90" spans="2:10" ht="18">
+    <row r="90" spans="2:10" ht="17.399999999999999">
       <c r="B90" s="41" t="s">
         <v>485</v>
       </c>
@@ -39814,7 +39805,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="91" spans="2:10" ht="18">
+    <row r="91" spans="2:10" ht="17.399999999999999">
       <c r="B91" s="41" t="s">
         <v>34</v>
       </c>
@@ -39841,7 +39832,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="92" spans="2:10" ht="18">
+    <row r="92" spans="2:10" ht="17.399999999999999">
       <c r="B92" s="41" t="s">
         <v>36</v>
       </c>
@@ -39868,7 +39859,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="93" spans="2:10" ht="18">
+    <row r="93" spans="2:10" ht="17.399999999999999">
       <c r="B93" s="35" t="s">
         <v>407</v>
       </c>
@@ -39895,7 +39886,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="94" spans="2:10" ht="18">
+    <row r="94" spans="2:10" ht="17.399999999999999">
       <c r="B94" s="35" t="s">
         <v>442</v>
       </c>
@@ -39922,7 +39913,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="95" spans="2:10" ht="18">
+    <row r="95" spans="2:10" ht="17.399999999999999">
       <c r="B95" s="41" t="s">
         <v>445</v>
       </c>
@@ -39949,7 +39940,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="96" spans="2:10" ht="18">
+    <row r="96" spans="2:10" ht="17.399999999999999">
       <c r="B96" s="41" t="s">
         <v>44</v>
       </c>
@@ -39976,7 +39967,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="97" spans="2:11" ht="18">
+    <row r="97" spans="2:11" ht="17.399999999999999">
       <c r="B97" s="35" t="s">
         <v>702</v>
       </c>
@@ -40003,7 +39994,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="98" spans="2:11" ht="18">
+    <row r="98" spans="2:11" ht="17.399999999999999">
       <c r="B98" s="35" t="s">
         <v>703</v>
       </c>
@@ -40030,10 +40021,10 @@
         <v>885</v>
       </c>
       <c r="K98" s="84" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="99" spans="2:11" ht="18">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11" ht="17.399999999999999">
       <c r="B99" s="35" t="s">
         <v>712</v>
       </c>
@@ -40060,7 +40051,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="100" spans="2:11" ht="18">
+    <row r="100" spans="2:11" ht="17.399999999999999">
       <c r="B100" s="35" t="s">
         <v>546</v>
       </c>
@@ -40087,7 +40078,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="101" spans="2:11" ht="18">
+    <row r="101" spans="2:11" ht="17.399999999999999">
       <c r="B101" s="35" t="s">
         <v>547</v>
       </c>
@@ -40114,7 +40105,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="102" spans="2:11" ht="18">
+    <row r="102" spans="2:11" ht="17.399999999999999">
       <c r="B102" s="35" t="s">
         <v>810</v>
       </c>
@@ -40144,7 +40135,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="103" spans="2:11" ht="18">
+    <row r="103" spans="2:11" ht="17.399999999999999">
       <c r="B103" s="35" t="s">
         <v>798</v>
       </c>
@@ -40163,10 +40154,10 @@
       </c>
       <c r="H103" s="112"/>
       <c r="K103" s="84" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="104" spans="2:11" ht="18">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="104" spans="2:11" ht="17.399999999999999">
       <c r="B104" s="35" t="s">
         <v>528</v>
       </c>
@@ -40193,7 +40184,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="105" spans="2:11" ht="18">
+    <row r="105" spans="2:11" ht="17.399999999999999">
       <c r="B105" s="35" t="s">
         <v>636</v>
       </c>
@@ -40220,7 +40211,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="106" spans="2:11" ht="18">
+    <row r="106" spans="2:11" ht="17.399999999999999">
       <c r="B106" s="35" t="s">
         <v>800</v>
       </c>
@@ -40247,7 +40238,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="107" spans="2:11" ht="18">
+    <row r="107" spans="2:11" ht="17.399999999999999">
       <c r="B107" s="35"/>
       <c r="C107" s="34"/>
       <c r="D107" s="35"/>
@@ -40257,7 +40248,7 @@
       <c r="H107" s="109"/>
       <c r="I107" s="9"/>
     </row>
-    <row r="108" spans="2:11" ht="18">
+    <row r="108" spans="2:11" ht="17.399999999999999">
       <c r="B108" s="35" t="s">
         <v>8</v>
       </c>
@@ -40284,7 +40275,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="109" spans="2:11" ht="18.75" thickBot="1">
+    <row r="109" spans="2:11" ht="18" thickBot="1">
       <c r="B109" s="35" t="s">
         <v>11</v>
       </c>
@@ -40338,7 +40329,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="111" spans="2:11" ht="18">
+    <row r="111" spans="2:11" ht="17.399999999999999">
       <c r="B111" s="35" t="s">
         <v>16</v>
       </c>
@@ -40365,7 +40356,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="112" spans="2:11" ht="18">
+    <row r="112" spans="2:11" ht="17.399999999999999">
       <c r="B112" s="35" t="s">
         <v>398</v>
       </c>
@@ -40392,7 +40383,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="113" spans="2:11" ht="18">
+    <row r="113" spans="2:11" ht="17.399999999999999">
       <c r="B113" s="35" t="s">
         <v>485</v>
       </c>
@@ -40419,7 +40410,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="114" spans="2:11" ht="18">
+    <row r="114" spans="2:11" ht="17.399999999999999">
       <c r="B114" s="35" t="s">
         <v>34</v>
       </c>
@@ -40446,7 +40437,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="115" spans="2:11" ht="18">
+    <row r="115" spans="2:11" ht="17.399999999999999">
       <c r="B115" s="35" t="s">
         <v>36</v>
       </c>
@@ -40473,7 +40464,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="116" spans="2:11" ht="18">
+    <row r="116" spans="2:11" ht="17.399999999999999">
       <c r="B116" s="35" t="s">
         <v>462</v>
       </c>
@@ -40500,7 +40491,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="117" spans="2:11" ht="18">
+    <row r="117" spans="2:11" ht="17.399999999999999">
       <c r="B117" s="35" t="s">
         <v>739</v>
       </c>
@@ -40527,10 +40518,10 @@
         <v>886</v>
       </c>
       <c r="K117" s="84" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="118" spans="2:11" ht="18">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="118" spans="2:11" ht="17.399999999999999">
       <c r="B118" s="35" t="s">
         <v>44</v>
       </c>
@@ -40557,7 +40548,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="119" spans="2:11" ht="18">
+    <row r="119" spans="2:11" ht="17.399999999999999">
       <c r="B119" s="35" t="s">
         <v>804</v>
       </c>
@@ -40584,10 +40575,10 @@
         <v>886</v>
       </c>
       <c r="K119" s="84" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="120" spans="2:11" ht="18">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="120" spans="2:11" ht="17.399999999999999">
       <c r="B120" s="35" t="s">
         <v>463</v>
       </c>
@@ -40614,7 +40605,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="121" spans="2:11" ht="18">
+    <row r="121" spans="2:11" ht="17.399999999999999">
       <c r="B121" s="35" t="s">
         <v>547</v>
       </c>
@@ -40641,7 +40632,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="122" spans="2:11" ht="18">
+    <row r="122" spans="2:11" ht="17.399999999999999">
       <c r="B122" s="35" t="s">
         <v>808</v>
       </c>
@@ -40668,7 +40659,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="123" spans="2:11" ht="18">
+    <row r="123" spans="2:11" ht="17.399999999999999">
       <c r="B123" s="35" t="s">
         <v>810</v>
       </c>
@@ -40686,7 +40677,7 @@
         <v>738</v>
       </c>
       <c r="H123" s="112" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="I123" s="84" t="s">
         <v>870</v>
@@ -40695,10 +40686,10 @@
         <v>886</v>
       </c>
       <c r="K123" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="124" spans="2:11" ht="18">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="124" spans="2:11" ht="17.399999999999999">
       <c r="B124" s="35" t="s">
         <v>532</v>
       </c>
@@ -40728,7 +40719,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="125" spans="2:11" ht="18">
+    <row r="125" spans="2:11" ht="17.399999999999999">
       <c r="B125" s="35" t="s">
         <v>533</v>
       </c>
@@ -40756,7 +40747,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="126" spans="2:11" ht="18">
+    <row r="126" spans="2:11" ht="17.399999999999999">
       <c r="B126" s="35"/>
       <c r="C126" s="34"/>
       <c r="D126" s="35"/>
@@ -40766,7 +40757,7 @@
       <c r="H126" s="109"/>
       <c r="I126" s="9"/>
     </row>
-    <row r="127" spans="2:11" ht="18">
+    <row r="127" spans="2:11" ht="17.399999999999999">
       <c r="B127" s="35" t="s">
         <v>8</v>
       </c>
@@ -40793,7 +40784,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="128" spans="2:11" ht="18">
+    <row r="128" spans="2:11" ht="17.399999999999999">
       <c r="B128" s="35" t="s">
         <v>11</v>
       </c>
@@ -40820,7 +40811,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="129" spans="2:10" ht="18">
+    <row r="129" spans="2:10" ht="17.399999999999999">
       <c r="B129" s="35" t="s">
         <v>13</v>
       </c>
@@ -40847,7 +40838,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="130" spans="2:10" ht="18">
+    <row r="130" spans="2:10" ht="17.399999999999999">
       <c r="B130" s="35" t="s">
         <v>16</v>
       </c>
@@ -40874,7 +40865,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="131" spans="2:10" ht="18">
+    <row r="131" spans="2:10" ht="17.399999999999999">
       <c r="B131" s="35" t="s">
         <v>398</v>
       </c>
@@ -40901,7 +40892,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="132" spans="2:10" ht="18">
+    <row r="132" spans="2:10" ht="17.399999999999999">
       <c r="B132" s="35" t="s">
         <v>485</v>
       </c>
@@ -40928,7 +40919,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="133" spans="2:10" ht="18">
+    <row r="133" spans="2:10" ht="17.399999999999999">
       <c r="B133" s="35" t="s">
         <v>503</v>
       </c>
@@ -40955,7 +40946,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="134" spans="2:10" ht="18">
+    <row r="134" spans="2:10" ht="17.399999999999999">
       <c r="B134" s="35" t="s">
         <v>34</v>
       </c>
@@ -40982,7 +40973,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="135" spans="2:10" ht="18">
+    <row r="135" spans="2:10" ht="17.399999999999999">
       <c r="B135" s="35" t="s">
         <v>36</v>
       </c>
@@ -41009,7 +41000,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="136" spans="2:10" ht="18">
+    <row r="136" spans="2:10" ht="17.399999999999999">
       <c r="B136" s="35" t="s">
         <v>559</v>
       </c>
@@ -41036,7 +41027,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="137" spans="2:10" ht="18">
+    <row r="137" spans="2:10" ht="17.399999999999999">
       <c r="B137" s="35" t="s">
         <v>44</v>
       </c>
@@ -41063,7 +41054,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="138" spans="2:10" ht="18">
+    <row r="138" spans="2:10" ht="17.399999999999999">
       <c r="B138" s="40" t="s">
         <v>470</v>
       </c>
@@ -41090,7 +41081,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="139" spans="2:10" ht="18">
+    <row r="139" spans="2:10" ht="17.399999999999999">
       <c r="B139" s="40" t="s">
         <v>736</v>
       </c>
@@ -41117,7 +41108,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="140" spans="2:10" ht="18">
+    <row r="140" spans="2:10" ht="17.399999999999999">
       <c r="B140" s="40" t="s">
         <v>463</v>
       </c>
@@ -41144,7 +41135,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="141" spans="2:10" ht="18">
+    <row r="141" spans="2:10" ht="17.399999999999999">
       <c r="B141" s="40"/>
       <c r="C141" s="34"/>
       <c r="D141" s="35"/>
@@ -41153,7 +41144,7 @@
       <c r="G141" s="37"/>
       <c r="H141" s="109"/>
     </row>
-    <row r="142" spans="2:10" ht="18">
+    <row r="142" spans="2:10" ht="17.399999999999999">
       <c r="B142" s="35" t="s">
         <v>8</v>
       </c>
@@ -41180,7 +41171,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="143" spans="2:10" ht="18">
+    <row r="143" spans="2:10" ht="17.399999999999999">
       <c r="B143" s="35" t="s">
         <v>11</v>
       </c>
@@ -41207,7 +41198,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="144" spans="2:10" ht="18.75" thickBot="1">
+    <row r="144" spans="2:10" ht="18" thickBot="1">
       <c r="B144" s="35" t="s">
         <v>13</v>
       </c>
@@ -41261,7 +41252,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="146" spans="2:11" ht="18">
+    <row r="146" spans="2:11" ht="17.399999999999999">
       <c r="B146" s="35" t="s">
         <v>34</v>
       </c>
@@ -41288,7 +41279,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="147" spans="2:11" ht="18">
+    <row r="147" spans="2:11" ht="17.399999999999999">
       <c r="B147" s="35" t="s">
         <v>36</v>
       </c>
@@ -41315,7 +41306,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="148" spans="2:11" ht="18">
+    <row r="148" spans="2:11" ht="17.399999999999999">
       <c r="B148" s="35" t="s">
         <v>44</v>
       </c>
@@ -41342,7 +41333,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="149" spans="2:11" ht="18">
+    <row r="149" spans="2:11" ht="17.399999999999999">
       <c r="B149" s="40" t="s">
         <v>470</v>
       </c>
@@ -41369,10 +41360,10 @@
         <v>888</v>
       </c>
       <c r="K149" s="84" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="150" spans="2:11" ht="18">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="150" spans="2:11" ht="17.399999999999999">
       <c r="B150" s="40" t="s">
         <v>463</v>
       </c>
@@ -41399,7 +41390,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="151" spans="2:11" ht="20.25">
+    <row r="151" spans="2:11" ht="20.399999999999999">
       <c r="B151" s="40"/>
       <c r="E151" s="88" t="s">
         <v>390</v>
@@ -41443,7 +41434,7 @@
       <c r="G155" s="14"/>
       <c r="H155" s="109"/>
     </row>
-    <row r="156" spans="2:11" ht="18">
+    <row r="156" spans="2:11" ht="17.399999999999999">
       <c r="B156" s="16"/>
       <c r="C156" s="19"/>
       <c r="D156" s="13"/>
@@ -41470,7 +41461,7 @@
       <c r="G159" s="14"/>
       <c r="H159" s="109"/>
     </row>
-    <row r="160" spans="2:11" ht="14.45" customHeight="1">
+    <row r="160" spans="2:11" ht="14.4" customHeight="1">
       <c r="B160" s="13"/>
       <c r="C160" s="15"/>
       <c r="D160" s="13"/>
@@ -41505,10 +41496,10 @@
     <row r="164" spans="2:8" ht="18" customHeight="1">
       <c r="D164" s="8"/>
     </row>
-    <row r="165" spans="2:8" ht="15.75">
+    <row r="165" spans="2:8" ht="15.6">
       <c r="C165" s="3"/>
     </row>
-    <row r="166" spans="2:8" ht="15.75">
+    <row r="166" spans="2:8" ht="15.6">
       <c r="B166" s="2"/>
       <c r="D166" s="2"/>
       <c r="E166" s="10"/>

</xml_diff>

<commit_message>
Omitting W 4x400 from here as better record of it in 2022 sheet
</commit_message>
<xml_diff>
--- a/2009_CnC_records.xlsx
+++ b/2009_CnC_records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9E2CD1-AD37-40C2-8448-931B264C743B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FAC80F-B083-478F-BE8F-0BD76DEF9EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="883" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="883" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Men" sheetId="10" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3598" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3597" uniqueCount="967">
   <si>
     <t>CAMBRIDGE &amp; COLERIDGE AC</t>
   </si>
@@ -2984,6 +2984,12 @@
   </si>
   <si>
     <t>Skipping this because PenIM35 age-group specific, also listed there</t>
+  </si>
+  <si>
+    <t>Complete with names in 2022 records so not using from here</t>
+  </si>
+  <si>
+    <t>No other record of this one so left in for now</t>
   </si>
 </sst>
 </file>
@@ -5840,9 +5846,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5880,7 +5886,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5986,7 +5992,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6128,7 +6134,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6141,7 +6147,7 @@
   </sheetPr>
   <dimension ref="B1:M1410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I29" sqref="I29:K29"/>
     </sheetView>
   </sheetViews>
@@ -16559,8 +16565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:M1396"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M58" sqref="M58"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="13.2"/>
@@ -17171,6 +17177,9 @@
       <c r="L26" s="84" t="s">
         <v>835</v>
       </c>
+      <c r="M26" s="84" t="s">
+        <v>966</v>
+      </c>
     </row>
     <row r="27" spans="2:13" ht="17.399999999999999">
       <c r="B27" s="35" t="s">
@@ -17191,14 +17200,11 @@
       <c r="I27" s="37" t="s">
         <v>675</v>
       </c>
-      <c r="J27" s="112" t="s">
-        <v>830</v>
-      </c>
-      <c r="K27" s="84" t="s">
-        <v>870</v>
-      </c>
-      <c r="L27" s="84" t="s">
-        <v>835</v>
+      <c r="J27" s="112"/>
+      <c r="K27" s="84"/>
+      <c r="L27" s="84"/>
+      <c r="M27" s="84" t="s">
+        <v>965</v>
       </c>
     </row>
     <row r="28" spans="2:13" ht="17.399999999999999">

</xml_diff>